<commit_message>
ADD - Brainstorm - SP Calculator
</commit_message>
<xml_diff>
--- a/Brainstorm.xlsx
+++ b/Brainstorm.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal@HDD\Game\DL\dragalia-data-track\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F49B5C-D507-4854-BD3E-F5723EB0642E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E29210D-6F37-4B39-B2CA-BE207F72EFBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32445" yWindow="3630" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{4CFB4A6A-60C6-4091-BCA5-480044B61D33}"/>
+    <workbookView xWindow="7575" yWindow="765" windowWidth="21135" windowHeight="12615" activeTab="1" xr2:uid="{4CFB4A6A-60C6-4091-BCA5-480044B61D33}"/>
   </bookViews>
   <sheets>
     <sheet name="Affliction" sheetId="1" r:id="rId1"/>
-    <sheet name="Equips" sheetId="6" r:id="rId2"/>
-    <sheet name="Steps" sheetId="4" r:id="rId3"/>
-    <sheet name="Damage" sheetId="7" r:id="rId4"/>
+    <sheet name="Rotation" sheetId="8" r:id="rId2"/>
+    <sheet name="Equips" sheetId="6" r:id="rId3"/>
+    <sheet name="Steps" sheetId="4" r:id="rId4"/>
+    <sheet name="Damage" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,8 +68,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="136">
   <si>
     <t>睡抗</t>
   </si>
@@ -377,13 +400,112 @@
   </si>
   <si>
     <t>濕身判定 (0 / 1)</t>
+  </si>
+  <si>
+    <t>武器種類</t>
+  </si>
+  <si>
+    <t>劍</t>
+  </si>
+  <si>
+    <t>短</t>
+  </si>
+  <si>
+    <t>斧</t>
+  </si>
+  <si>
+    <t>槍</t>
+  </si>
+  <si>
+    <t>弓</t>
+  </si>
+  <si>
+    <t>補</t>
+  </si>
+  <si>
+    <t>長銃</t>
+  </si>
+  <si>
+    <t>短銃</t>
+  </si>
+  <si>
+    <t>散銃</t>
+  </si>
+  <si>
+    <t>EX</t>
+  </si>
+  <si>
+    <t>護符</t>
+  </si>
+  <si>
+    <t>連組</t>
+  </si>
+  <si>
+    <t>技能資訊</t>
+  </si>
+  <si>
+    <t>計算結果</t>
+  </si>
+  <si>
+    <t>一套 SP</t>
+  </si>
+  <si>
+    <t>SP 表 (Combo 為累加)</t>
+  </si>
+  <si>
+    <t>原始 SP 表 (Combo 為累加)</t>
+  </si>
+  <si>
+    <t>SP +%</t>
+  </si>
+  <si>
+    <t>SP 回流%</t>
+  </si>
+  <si>
+    <t>S1 SP</t>
+  </si>
+  <si>
+    <t>S1 實際 SP</t>
+  </si>
+  <si>
+    <t>S2 SP</t>
+  </si>
+  <si>
+    <t>S1 輪轉</t>
+  </si>
+  <si>
+    <t>S2 輪轉</t>
+  </si>
+  <si>
+    <t>S1 補刀 SP</t>
+  </si>
+  <si>
+    <t>S2 補刀 SP</t>
+  </si>
+  <si>
+    <t>S2 實際 SP</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,8 +565,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="39">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,8 +827,38 @@
         <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF240000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000C24"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF030024"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -879,25 +1063,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1102,6 +1285,120 @@
     <xf numFmtId="0" fontId="6" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="23" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="23" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="23" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="28" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="30" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="30" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="30" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="32" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="32" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="35" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="35" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1114,27 +1411,12 @@
     <xf numFmtId="3" fontId="8" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1150,103 +1432,112 @@
     <xf numFmtId="0" fontId="6" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="35" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="35" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="30" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="30" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="30" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="32" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="32" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="23" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="23" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="23" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="28" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="39" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="39" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="39" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="40" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="42" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="41" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="43" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="43" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1258,16 +1549,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF030024"/>
+      <color rgb="FF003217"/>
+      <color rgb="FF240000"/>
+      <color rgb="FF323100"/>
+      <color rgb="FF000C24"/>
       <color rgb="FF242300"/>
-      <color rgb="FF000C24"/>
-      <color rgb="FF240000"/>
       <color rgb="FF140000"/>
       <color rgb="FF0E2234"/>
       <color rgb="FF320000"/>
       <color rgb="FF1B0C26"/>
-      <color rgb="FF003217"/>
-      <color rgb="FF323100"/>
-      <color rgb="FF001132"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1603,191 +1894,936 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="10.85546875" style="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="4"/>
-    <col min="6" max="6" width="18.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="1"/>
-    <col min="8" max="9" width="13.28515625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="3" width="10.85546875" style="118"/>
+    <col min="4" max="4" width="13.28515625" style="118" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="120"/>
+    <col min="6" max="6" width="18.42578125" style="118" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="118"/>
+    <col min="8" max="9" width="13.28515625" style="118" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="118"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="119">
         <v>0.99</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="118" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="118" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="119">
         <v>0.99</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="120">
         <f>B4-B2</f>
         <v>0.81</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="121">
         <f>VLOOKUP(H2,$D:$E,2,FALSE)*VLOOKUP(I2,$D:$E,2,FALSE)</f>
         <v>8.9100000000000082E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="119">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="120">
         <f>1-E2</f>
         <v>0.18999999999999995</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="121">
         <f>VLOOKUP(H3,$D:$E,2,FALSE)*VLOOKUP(I3,$D:$E,2,FALSE)</f>
         <v>0.16839900000000016</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="119">
         <v>1.8</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="120">
         <f>1-E5</f>
         <v>0.96389999999999998</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="121">
         <f>VLOOKUP(H4,$D:$E,2,FALSE)*VLOOKUP(I4,$D:$E,2,FALSE)</f>
         <v>0.20039481000000017</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="120">
         <f>E3*E3</f>
         <v>3.6099999999999979E-2</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="121">
         <f>VLOOKUP(H5,$D:$E,2,FALSE)*VLOOKUP(I5,$D:$E,2,FALSE)</f>
         <v>9.801000000000018E-3</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="120">
         <f>B3-B1</f>
         <v>0.1100000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="120">
         <f>1-E6</f>
         <v>0.8899999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="120">
         <f>1-E9</f>
         <v>0.2079000000000002</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="118" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="120">
         <f>E7*E7</f>
         <v>0.7920999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="120">
         <f>E6*E6</f>
         <v>1.2100000000000022E-2</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B260D6A6-975E-4594-902D-33C279C7CA35}">
+  <dimension ref="A1:V13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="14" width="5.85546875" style="118" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="148" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" style="150" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" style="124" customWidth="1"/>
+    <col min="18" max="18" width="5.85546875" style="132" customWidth="1"/>
+    <col min="19" max="19" width="11" style="125" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" style="13" customWidth="1"/>
+    <col min="21" max="21" width="11" style="130" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" style="15" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="118"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="136" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="136" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="137"/>
+      <c r="N1" s="138"/>
+      <c r="O1" s="146" t="s">
+        <v>122</v>
+      </c>
+      <c r="P1" s="147"/>
+      <c r="Q1" s="139" t="s">
+        <v>121</v>
+      </c>
+      <c r="R1" s="140"/>
+      <c r="S1" s="141" t="s">
+        <v>116</v>
+      </c>
+      <c r="T1" s="142"/>
+      <c r="U1" s="143" t="s">
+        <v>117</v>
+      </c>
+      <c r="V1" s="144"/>
+    </row>
+    <row r="2" spans="1:22" s="122" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="129" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="127" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="127" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="127" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" s="127" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" s="128" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="129" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="127" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="127" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2" s="127" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" s="127" t="s">
+        <v>135</v>
+      </c>
+      <c r="N2" s="128" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="148" t="s">
+        <v>113</v>
+      </c>
+      <c r="P2" s="149">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="124" t="s">
+        <v>113</v>
+      </c>
+      <c r="R2" s="131">
+        <v>0.15</v>
+      </c>
+      <c r="S2" s="125" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="12"/>
+      <c r="U2" s="133" t="s">
+        <v>118</v>
+      </c>
+      <c r="V2" s="134">
+        <f>VLOOKUP(T3,$H$3:$M$13,6,FALSE)</f>
+        <v>2464.8000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="126">
+        <v>150</v>
+      </c>
+      <c r="C3" s="126">
+        <v>300</v>
+      </c>
+      <c r="D3" s="126">
+        <v>496</v>
+      </c>
+      <c r="E3" s="126">
+        <v>761</v>
+      </c>
+      <c r="F3" s="126">
+        <v>1152</v>
+      </c>
+      <c r="G3" s="123">
+        <v>345</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" s="126">
+        <f>B3 * (1+SUM($R:$R))</f>
+        <v>237</v>
+      </c>
+      <c r="J3" s="126">
+        <f t="shared" ref="J3:J13" si="0">C3 * (1+SUM($R:$R))</f>
+        <v>474</v>
+      </c>
+      <c r="K3" s="126">
+        <f>D3 * (1+SUM($R:$R))</f>
+        <v>783.68000000000006</v>
+      </c>
+      <c r="L3" s="126">
+        <f>E3 * (1+SUM($R:$R))</f>
+        <v>1202.3800000000001</v>
+      </c>
+      <c r="M3" s="126">
+        <f>F3 * (1+SUM($R:$R))</f>
+        <v>1820.16</v>
+      </c>
+      <c r="N3" s="123">
+        <f t="shared" ref="N3:N13" si="1">G3 * (1+SUM($R:$R))</f>
+        <v>545.1</v>
+      </c>
+      <c r="O3" s="148" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="149">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="124" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="131">
+        <v>0.35</v>
+      </c>
+      <c r="S3" s="125" t="s">
+        <v>103</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="U3" s="133" t="s">
+        <v>128</v>
+      </c>
+      <c r="V3" s="134">
+        <f>MOD(T6, V2)</f>
+        <v>2305.1999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="126">
+        <v>130</v>
+      </c>
+      <c r="C4" s="126">
+        <v>260</v>
+      </c>
+      <c r="D4" s="126">
+        <v>480</v>
+      </c>
+      <c r="E4" s="126">
+        <v>840</v>
+      </c>
+      <c r="F4" s="126">
+        <v>1740</v>
+      </c>
+      <c r="G4" s="123">
+        <v>200</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="126">
+        <f t="shared" ref="I4:I13" si="2">B4 * (1+SUM($R:$R))</f>
+        <v>205.4</v>
+      </c>
+      <c r="J4" s="126">
+        <f t="shared" si="0"/>
+        <v>410.8</v>
+      </c>
+      <c r="K4" s="126">
+        <f>D4 * (1+SUM($R:$R))</f>
+        <v>758.40000000000009</v>
+      </c>
+      <c r="L4" s="126">
+        <f>E4 * (1+SUM($R:$R))</f>
+        <v>1327.2</v>
+      </c>
+      <c r="M4" s="126">
+        <f>F4 * (1+SUM($R:$R))</f>
+        <v>2749.2000000000003</v>
+      </c>
+      <c r="N4" s="123">
+        <f t="shared" si="1"/>
+        <v>316</v>
+      </c>
+      <c r="O4" s="148" t="s">
+        <v>114</v>
+      </c>
+      <c r="P4" s="149">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="124" t="s">
+        <v>114</v>
+      </c>
+      <c r="R4" s="131">
+        <v>0.08</v>
+      </c>
+      <c r="S4" s="125" t="s">
+        <v>123</v>
+      </c>
+      <c r="T4" s="13">
+        <v>4770</v>
+      </c>
+      <c r="U4" s="133" t="s">
+        <v>129</v>
+      </c>
+      <c r="V4" s="134">
+        <f>MOD(T7, V2)</f>
+        <v>1870.3999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="126">
+        <v>144</v>
+      </c>
+      <c r="C5" s="126">
+        <v>288</v>
+      </c>
+      <c r="D5" s="126">
+        <v>552</v>
+      </c>
+      <c r="E5" s="126">
+        <v>840</v>
+      </c>
+      <c r="F5" s="126">
+        <v>1320</v>
+      </c>
+      <c r="G5" s="123">
+        <v>288</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="126">
+        <f t="shared" si="2"/>
+        <v>227.52</v>
+      </c>
+      <c r="J5" s="126">
+        <f t="shared" si="0"/>
+        <v>455.04</v>
+      </c>
+      <c r="K5" s="126">
+        <f>D5 * (1+SUM($R:$R))</f>
+        <v>872.16000000000008</v>
+      </c>
+      <c r="L5" s="126">
+        <f>E5 * (1+SUM($R:$R))</f>
+        <v>1327.2</v>
+      </c>
+      <c r="M5" s="126">
+        <f>F5 * (1+SUM($R:$R))</f>
+        <v>2085.6</v>
+      </c>
+      <c r="N5" s="123">
+        <f t="shared" si="1"/>
+        <v>455.04</v>
+      </c>
+      <c r="O5" s="148" t="s">
+        <v>115</v>
+      </c>
+      <c r="P5" s="149">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="124" t="s">
+        <v>115</v>
+      </c>
+      <c r="R5" s="131">
+        <v>0</v>
+      </c>
+      <c r="S5" s="125" t="s">
+        <v>125</v>
+      </c>
+      <c r="T5" s="13">
+        <v>6800</v>
+      </c>
+      <c r="U5" s="135" t="s">
+        <v>126</v>
+      </c>
+      <c r="V5" s="145" t="str" cm="1">
+        <f t="array" ref="V5">ROUNDDOWN(T6/V2, 0) + IF(AND(V3 &gt; VLOOKUP(T3,H3:N13,5,0), V3 &lt; VLOOKUP(T3,H3:N13,6,0)), 1, 0) &amp; _xlfn.IFS(V3 &lt; VLOOKUP(T3,$H3:N13,7,FALSE), " + FS", VLOOKUP($T$3,H3:N13,2,0) &gt; V3, " + C1", VLOOKUP(T3,H3:N13,3,0) &gt; V3, " + C2", VLOOKUP(T3,H3:N13,4,0) &gt; V3, " + C3", VLOOKUP(T3,H3:N13,5,0) &gt; V3, " + C4",TRUE,"")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="126">
+        <v>200</v>
+      </c>
+      <c r="C6" s="126">
+        <v>440</v>
+      </c>
+      <c r="D6" s="126">
+        <v>800</v>
+      </c>
+      <c r="E6" s="126">
+        <v>1180</v>
+      </c>
+      <c r="F6" s="126">
+        <v>1600</v>
+      </c>
+      <c r="G6" s="123">
+        <v>300</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" s="126">
+        <f t="shared" si="2"/>
+        <v>316</v>
+      </c>
+      <c r="J6" s="126">
+        <f t="shared" si="0"/>
+        <v>695.2</v>
+      </c>
+      <c r="K6" s="126">
+        <f>D6 * (1+SUM($R:$R))</f>
+        <v>1264</v>
+      </c>
+      <c r="L6" s="126">
+        <f>E6 * (1+SUM($R:$R))</f>
+        <v>1864.4</v>
+      </c>
+      <c r="M6" s="126">
+        <f>F6 * (1+SUM($R:$R))</f>
+        <v>2528</v>
+      </c>
+      <c r="N6" s="123">
+        <f t="shared" si="1"/>
+        <v>474</v>
+      </c>
+      <c r="S6" s="151" t="s">
+        <v>124</v>
+      </c>
+      <c r="T6" s="152">
+        <f>T4 * (1 - SUM(P:P))</f>
+        <v>4770</v>
+      </c>
+      <c r="U6" s="153" t="s">
+        <v>127</v>
+      </c>
+      <c r="V6" s="145" t="str" cm="1">
+        <f t="array" ref="V6">ROUNDDOWN(T7/V2, 0) + IF(AND(V4 &gt; VLOOKUP(T3,H3:N13,5,0), V4 &lt; VLOOKUP(T3,H3:N13,6,0)), 1, 0) &amp; _xlfn.IFS(V4 &lt; VLOOKUP(T3,$H3:N13,7,FALSE), " + FS", VLOOKUP($T$3,H3:N13,2,0) &gt; V4, " + C1", VLOOKUP(T3,H3:N13,3,0) &gt; V4, " + C2", VLOOKUP(T3,H3:N13,4,0) &gt; V4, " + C3", VLOOKUP(T3,H3:N13,5,0) &gt; V4, " + C4",TRUE,"")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="126">
+        <v>120</v>
+      </c>
+      <c r="C7" s="126">
+        <v>360</v>
+      </c>
+      <c r="D7" s="126">
+        <v>480</v>
+      </c>
+      <c r="E7" s="126">
+        <v>960</v>
+      </c>
+      <c r="F7" s="126">
+        <v>1560</v>
+      </c>
+      <c r="G7" s="123">
+        <v>400</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I7" s="126">
+        <f t="shared" si="2"/>
+        <v>189.60000000000002</v>
+      </c>
+      <c r="J7" s="126">
+        <f t="shared" si="0"/>
+        <v>568.80000000000007</v>
+      </c>
+      <c r="K7" s="126">
+        <f>D7 * (1+SUM($R:$R))</f>
+        <v>758.40000000000009</v>
+      </c>
+      <c r="L7" s="126">
+        <f>E7 * (1+SUM($R:$R))</f>
+        <v>1516.8000000000002</v>
+      </c>
+      <c r="M7" s="126">
+        <f>F7 * (1+SUM($R:$R))</f>
+        <v>2464.8000000000002</v>
+      </c>
+      <c r="N7" s="123">
+        <f t="shared" si="1"/>
+        <v>632</v>
+      </c>
+      <c r="S7" s="151" t="s">
+        <v>130</v>
+      </c>
+      <c r="T7" s="152">
+        <f>T5 * (1 - SUM(P:P))</f>
+        <v>6800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="126">
+        <v>184</v>
+      </c>
+      <c r="C8" s="126">
+        <v>276</v>
+      </c>
+      <c r="D8" s="126">
+        <v>552</v>
+      </c>
+      <c r="E8" s="126">
+        <v>966</v>
+      </c>
+      <c r="F8" s="126">
+        <v>1495</v>
+      </c>
+      <c r="G8" s="123">
+        <v>460</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="126">
+        <f t="shared" si="2"/>
+        <v>290.72000000000003</v>
+      </c>
+      <c r="J8" s="126">
+        <f t="shared" si="0"/>
+        <v>436.08000000000004</v>
+      </c>
+      <c r="K8" s="126">
+        <f>D8 * (1+SUM($R:$R))</f>
+        <v>872.16000000000008</v>
+      </c>
+      <c r="L8" s="126">
+        <f>E8 * (1+SUM($R:$R))</f>
+        <v>1526.28</v>
+      </c>
+      <c r="M8" s="126">
+        <f>F8 * (1+SUM($R:$R))</f>
+        <v>2362.1</v>
+      </c>
+      <c r="N8" s="123">
+        <f t="shared" si="1"/>
+        <v>726.80000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="126">
+        <v>130</v>
+      </c>
+      <c r="C9" s="126">
+        <v>330</v>
+      </c>
+      <c r="D9" s="126">
+        <v>570</v>
+      </c>
+      <c r="E9" s="126">
+        <v>1000</v>
+      </c>
+      <c r="F9" s="126">
+        <v>1600</v>
+      </c>
+      <c r="G9" s="123">
+        <v>400</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="126">
+        <f t="shared" si="2"/>
+        <v>205.4</v>
+      </c>
+      <c r="J9" s="126">
+        <f t="shared" si="0"/>
+        <v>521.4</v>
+      </c>
+      <c r="K9" s="126">
+        <f>D9 * (1+SUM($R:$R))</f>
+        <v>900.6</v>
+      </c>
+      <c r="L9" s="126">
+        <f>E9 * (1+SUM($R:$R))</f>
+        <v>1580</v>
+      </c>
+      <c r="M9" s="126">
+        <f>F9 * (1+SUM($R:$R))</f>
+        <v>2528</v>
+      </c>
+      <c r="N9" s="123">
+        <f t="shared" si="1"/>
+        <v>632</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="126">
+        <v>232</v>
+      </c>
+      <c r="C10" s="126">
+        <v>464</v>
+      </c>
+      <c r="D10" s="126">
+        <v>812</v>
+      </c>
+      <c r="E10" s="126">
+        <v>1276</v>
+      </c>
+      <c r="F10" s="126">
+        <v>1972</v>
+      </c>
+      <c r="G10" s="123">
+        <v>580</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="126">
+        <f t="shared" si="2"/>
+        <v>366.56</v>
+      </c>
+      <c r="J10" s="126">
+        <f t="shared" si="0"/>
+        <v>733.12</v>
+      </c>
+      <c r="K10" s="126">
+        <f>D10 * (1+SUM($R:$R))</f>
+        <v>1282.96</v>
+      </c>
+      <c r="L10" s="126">
+        <f>E10 * (1+SUM($R:$R))</f>
+        <v>2016.0800000000002</v>
+      </c>
+      <c r="M10" s="126">
+        <f>F10 * (1+SUM($R:$R))</f>
+        <v>3115.76</v>
+      </c>
+      <c r="N10" s="123">
+        <f t="shared" si="1"/>
+        <v>916.40000000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="126">
+        <v>545</v>
+      </c>
+      <c r="C11" s="126">
+        <v>1090</v>
+      </c>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="123">
+        <v>400</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="I11" s="126">
+        <f t="shared" si="2"/>
+        <v>861.1</v>
+      </c>
+      <c r="J11" s="126">
+        <f t="shared" si="0"/>
+        <v>1722.2</v>
+      </c>
+      <c r="K11" s="126"/>
+      <c r="L11" s="126"/>
+      <c r="M11" s="126"/>
+      <c r="N11" s="123">
+        <f t="shared" si="1"/>
+        <v>632</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="126">
+        <v>464</v>
+      </c>
+      <c r="C12" s="126">
+        <v>928</v>
+      </c>
+      <c r="D12" s="126"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="123">
+        <v>400</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I12" s="126">
+        <f t="shared" si="2"/>
+        <v>733.12</v>
+      </c>
+      <c r="J12" s="126">
+        <f t="shared" si="0"/>
+        <v>1466.24</v>
+      </c>
+      <c r="K12" s="126"/>
+      <c r="L12" s="126"/>
+      <c r="M12" s="126"/>
+      <c r="N12" s="123">
+        <f t="shared" si="1"/>
+        <v>632</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" s="126">
+        <v>300</v>
+      </c>
+      <c r="C13" s="126">
+        <v>764</v>
+      </c>
+      <c r="D13" s="126">
+        <v>1228</v>
+      </c>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
+      <c r="G13" s="123">
+        <v>400</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I13" s="126">
+        <f t="shared" si="2"/>
+        <v>474</v>
+      </c>
+      <c r="J13" s="126">
+        <f t="shared" si="0"/>
+        <v>1207.1200000000001</v>
+      </c>
+      <c r="K13" s="126">
+        <f>D13 * (1+SUM($R:$R))</f>
+        <v>1940.24</v>
+      </c>
+      <c r="L13" s="126"/>
+      <c r="M13" s="126"/>
+      <c r="N13" s="123">
+        <f t="shared" si="1"/>
+        <v>632</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="O1:P1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6E1F14-9A03-4157-97E0-B9040F803B9F}">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -1797,209 +2833,209 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="5" width="16.5703125" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="5" width="16.5703125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="11" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2008,7 +3044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F18558-26E5-406D-8DCA-7A8488B0D961}">
   <dimension ref="A1:M13"/>
   <sheetViews>
@@ -2018,190 +3054,190 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="5" style="8" customWidth="1"/>
-    <col min="3" max="66" width="4.5703125" style="6" customWidth="1"/>
-    <col min="67" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="7.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="5" style="4" customWidth="1"/>
+    <col min="3" max="66" width="4.5703125" style="2" customWidth="1"/>
+    <col min="67" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="22">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="10" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:13" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="10" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="M3" s="10" t="s">
+    <row r="3" spans="1:13" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="M3" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="10" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:13" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="10">
+      <c r="B4" s="4"/>
+      <c r="C4" s="6">
         <v>1</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="6">
         <v>3</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="6">
         <v>4</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="12" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:13" s="8" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="L5" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="12" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="L6" s="12" t="s">
+    <row r="6" spans="1:13" s="8" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="L6" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="12" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:13" s="8" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="12">
+      <c r="B7" s="4"/>
+      <c r="C7" s="8">
         <v>1</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="8">
         <v>3</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="8">
         <v>4</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:13" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="F9" s="23" t="s">
+    <row r="9" spans="1:13" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="F9" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:13" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="D10" s="13">
+      <c r="B10" s="4"/>
+      <c r="D10" s="9">
         <v>3</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="13">
+      <c r="F10" s="19"/>
+      <c r="G10" s="9">
         <v>4</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="19" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:13" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="I11" s="20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="19" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:13" s="19" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+    <row r="12" spans="1:13" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="19">
+      <c r="B13" s="4"/>
+      <c r="C13" s="15">
         <v>1</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="15">
         <v>3</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="15">
         <v>4</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="15">
         <v>5</v>
       </c>
     </row>
@@ -2210,554 +3246,530 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFF6CA3-18A6-4987-88AD-5768B35D8A0C}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E11" sqref="E11"/>
+      <selection pane="topRight" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="71"/>
-    <col min="2" max="2" width="19" style="72" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="64" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="27" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="27"/>
-    <col min="6" max="6" width="11.28515625" style="27" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="27"/>
+    <col min="1" max="1" width="9.140625" style="67"/>
+    <col min="2" max="2" width="19" style="68" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="60" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="23"/>
+    <col min="6" max="6" width="11.28515625" style="23" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="120" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="121"/>
-      <c r="E1" s="120" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="121"/>
+      <c r="F1" s="72"/>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="52">
+      <c r="B2" s="74"/>
+      <c r="C2" s="48">
         <f>5/3</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="25">
         <f>C2</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="E2" s="28">
+      <c r="E2" s="24">
         <f>5/3</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="25">
         <f>E2</f>
         <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="52">
+      <c r="B3" s="74"/>
+      <c r="C3" s="48">
         <v>0</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="25">
         <f>1-C3</f>
         <v>1</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="24">
         <v>0</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="25">
         <f>1-E3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+    <row r="4" spans="1:6" s="28" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="53">
+      <c r="C4" s="49">
         <v>6016</v>
       </c>
-      <c r="D4" s="109">
+      <c r="D4" s="78">
         <f>(C4/(1+C5)*(1+C5+C6)*(1+C7)*(1+C8))</f>
         <v>16279.295999999998</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="27">
         <v>5348</v>
       </c>
-      <c r="F4" s="109">
+      <c r="F4" s="78">
         <f>(E4/(1+E5)*(1+E5+E6)*(1+E7)*(1+E8))</f>
         <v>14471.688000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="82"/>
-      <c r="B5" s="65" t="s">
+    <row r="5" spans="1:6" s="28" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="76"/>
+      <c r="B5" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="50">
         <v>0.35</v>
       </c>
-      <c r="D5" s="110"/>
-      <c r="E5" s="33">
+      <c r="D5" s="79"/>
+      <c r="E5" s="29">
         <v>0.2</v>
       </c>
-      <c r="F5" s="110"/>
-    </row>
-    <row r="6" spans="1:6" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="82"/>
-      <c r="B6" s="65" t="s">
+      <c r="F5" s="79"/>
+    </row>
+    <row r="6" spans="1:6" s="28" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="76"/>
+      <c r="B6" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="55">
+      <c r="C6" s="51">
         <v>0</v>
       </c>
-      <c r="D6" s="110"/>
-      <c r="E6" s="34">
+      <c r="D6" s="79"/>
+      <c r="E6" s="30">
         <v>0</v>
       </c>
-      <c r="F6" s="110"/>
-    </row>
-    <row r="7" spans="1:6" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="82"/>
-      <c r="B7" s="65" t="s">
+      <c r="F6" s="79"/>
+    </row>
+    <row r="7" spans="1:6" s="28" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="76"/>
+      <c r="B7" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="55">
+      <c r="C7" s="51">
         <v>1.46</v>
       </c>
-      <c r="D7" s="110"/>
-      <c r="E7" s="34">
+      <c r="D7" s="79"/>
+      <c r="E7" s="30">
         <v>1.46</v>
       </c>
-      <c r="F7" s="110"/>
-    </row>
-    <row r="8" spans="1:6" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="83"/>
-      <c r="B8" s="65" t="s">
+      <c r="F7" s="79"/>
+    </row>
+    <row r="8" spans="1:6" s="28" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="77"/>
+      <c r="B8" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="55">
+      <c r="C8" s="51">
         <v>0.1</v>
       </c>
-      <c r="D8" s="111"/>
-      <c r="E8" s="34">
+      <c r="D8" s="80"/>
+      <c r="E8" s="30">
         <v>0.1</v>
       </c>
-      <c r="F8" s="111"/>
-    </row>
-    <row r="9" spans="1:6" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="112" t="s">
+      <c r="F8" s="80"/>
+    </row>
+    <row r="9" spans="1:6" s="33" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="113"/>
-      <c r="C9" s="56">
+      <c r="B9" s="82"/>
+      <c r="C9" s="52">
         <v>36</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="32">
         <f>C9</f>
         <v>36</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="31">
         <v>36</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F9" s="32">
         <f>E9</f>
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="114" t="s">
+    <row r="10" spans="1:6" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="57">
+      <c r="C10" s="53">
         <v>1</v>
       </c>
-      <c r="D10" s="116">
+      <c r="D10" s="85">
         <f>1+((0.7+C11)*C10)</f>
         <v>2.15</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="34">
         <v>1</v>
       </c>
-      <c r="F10" s="116">
+      <c r="F10" s="85">
         <f>1+((0.7+E11)*E10)</f>
         <v>2.15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="115"/>
-      <c r="B11" s="66" t="s">
+    <row r="11" spans="1:6" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="84"/>
+      <c r="B11" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="58">
+      <c r="C11" s="54">
         <v>0.45</v>
       </c>
-      <c r="D11" s="117"/>
-      <c r="E11" s="40">
+      <c r="D11" s="86"/>
+      <c r="E11" s="36">
         <v>0.45</v>
       </c>
-      <c r="F11" s="117"/>
-    </row>
-    <row r="12" spans="1:6" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="99" t="s">
+      <c r="F11" s="86"/>
+    </row>
+    <row r="12" spans="1:6" s="38" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="59">
+      <c r="C12" s="55">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D12" s="102">
+      <c r="D12" s="90">
         <f>(1+C12+C13)*(1+C14)*(1+C15)</f>
         <v>2.415</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="37">
         <v>1.3</v>
       </c>
-      <c r="F12" s="102">
+      <c r="F12" s="90">
         <f>(1+E12+E13)*(1+E14)*(1+E15)</f>
         <v>2.6449999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="100"/>
-      <c r="B13" s="67" t="s">
+    <row r="13" spans="1:6" s="38" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="88"/>
+      <c r="B13" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="59">
+      <c r="C13" s="55">
         <v>0</v>
       </c>
-      <c r="D13" s="103"/>
-      <c r="E13" s="41">
+      <c r="D13" s="91"/>
+      <c r="E13" s="37">
         <v>0</v>
       </c>
-      <c r="F13" s="103"/>
-    </row>
-    <row r="14" spans="1:6" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="100"/>
-      <c r="B14" s="67" t="s">
+      <c r="F13" s="91"/>
+    </row>
+    <row r="14" spans="1:6" s="38" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="88"/>
+      <c r="B14" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="59">
+      <c r="C14" s="55">
         <v>0.15</v>
       </c>
-      <c r="D14" s="103"/>
-      <c r="E14" s="41">
+      <c r="D14" s="91"/>
+      <c r="E14" s="37">
         <v>0.15</v>
       </c>
-      <c r="F14" s="103"/>
-    </row>
-    <row r="15" spans="1:6" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="101"/>
-      <c r="B15" s="67" t="s">
+      <c r="F14" s="91"/>
+    </row>
+    <row r="15" spans="1:6" s="38" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="89"/>
+      <c r="B15" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="59">
+      <c r="C15" s="55">
         <v>0</v>
       </c>
-      <c r="D15" s="104"/>
-      <c r="E15" s="41">
+      <c r="D15" s="92"/>
+      <c r="E15" s="37">
         <v>0</v>
       </c>
-      <c r="F15" s="104"/>
-    </row>
-    <row r="16" spans="1:6" s="44" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="105" t="s">
+      <c r="F15" s="92"/>
+    </row>
+    <row r="16" spans="1:6" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="60">
+      <c r="C16" s="56">
         <v>0</v>
       </c>
-      <c r="D16" s="107">
+      <c r="D16" s="95">
         <f>(1+C16)*(1+C17)</f>
         <v>1.2</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="39">
         <v>0</v>
       </c>
-      <c r="F16" s="107">
+      <c r="F16" s="95">
         <f>(1+E16)*(1+E17)</f>
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="44" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="106"/>
-      <c r="B17" s="68" t="s">
+    <row r="17" spans="1:6" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="94"/>
+      <c r="B17" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="60">
+      <c r="C17" s="56">
         <v>0.2</v>
       </c>
-      <c r="D17" s="108"/>
-      <c r="E17" s="43">
+      <c r="D17" s="96"/>
+      <c r="E17" s="39">
         <v>0.2</v>
       </c>
-      <c r="F17" s="108"/>
-    </row>
-    <row r="18" spans="1:6" s="46" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="89" t="s">
+      <c r="F17" s="96"/>
+    </row>
+    <row r="18" spans="1:6" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="69" t="s">
+      <c r="B18" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="61">
+      <c r="C18" s="57">
         <v>1.5</v>
       </c>
-      <c r="D18" s="91">
+      <c r="D18" s="99">
         <f>C18+C19</f>
         <v>1.5</v>
       </c>
-      <c r="E18" s="45">
+      <c r="E18" s="41">
         <v>1.5</v>
       </c>
-      <c r="F18" s="91">
+      <c r="F18" s="99">
         <f>E18+E19</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="46" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="90"/>
-      <c r="B19" s="69" t="s">
+    <row r="19" spans="1:6" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="98"/>
+      <c r="B19" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="62">
+      <c r="C19" s="58">
         <v>0</v>
       </c>
-      <c r="D19" s="92"/>
-      <c r="E19" s="47">
+      <c r="D19" s="100"/>
+      <c r="E19" s="43">
         <v>0</v>
       </c>
-      <c r="F19" s="92"/>
-    </row>
-    <row r="20" spans="1:6" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="93" t="s">
+      <c r="F19" s="100"/>
+    </row>
+    <row r="20" spans="1:6" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="101" t="s">
         <v>98</v>
       </c>
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="63">
+      <c r="C20" s="59">
         <v>0</v>
       </c>
-      <c r="D20" s="96">
+      <c r="D20" s="104">
         <f>1+C20*(0.2+C21+C22)</f>
         <v>1</v>
       </c>
-      <c r="E20" s="48">
+      <c r="E20" s="44">
         <v>0</v>
       </c>
-      <c r="F20" s="96">
+      <c r="F20" s="104">
         <f>1+E20*(0.2+E21+E22)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="94"/>
-      <c r="B21" s="70" t="s">
+    <row r="21" spans="1:6" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="102"/>
+      <c r="B21" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="63">
+      <c r="C21" s="59">
         <v>0.5</v>
       </c>
-      <c r="D21" s="97"/>
-      <c r="E21" s="48">
+      <c r="D21" s="105"/>
+      <c r="E21" s="44">
         <v>0.5</v>
       </c>
-      <c r="F21" s="97"/>
-    </row>
-    <row r="22" spans="1:6" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="95"/>
-      <c r="B22" s="70" t="s">
+      <c r="F21" s="105"/>
+    </row>
+    <row r="22" spans="1:6" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="103"/>
+      <c r="B22" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="63">
+      <c r="C22" s="59">
         <v>0</v>
       </c>
-      <c r="D22" s="98"/>
-      <c r="E22" s="48">
+      <c r="D22" s="106"/>
+      <c r="E22" s="44">
         <v>0</v>
       </c>
-      <c r="F22" s="98"/>
+      <c r="F22" s="106"/>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="78"/>
-      <c r="C23" s="52">
+      <c r="B23" s="74"/>
+      <c r="C23" s="48">
         <v>1</v>
       </c>
-      <c r="D23" s="30">
+      <c r="D23" s="26">
         <f>C23</f>
         <v>1</v>
       </c>
-      <c r="E23" s="28">
+      <c r="E23" s="24">
         <v>1</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F23" s="26">
         <f>E23</f>
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="79" t="s">
+    <row r="24" spans="1:6" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="111" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="80"/>
-      <c r="C24" s="63">
+      <c r="B24" s="112"/>
+      <c r="C24" s="59">
         <v>10</v>
       </c>
-      <c r="D24" s="50">
+      <c r="D24" s="46">
         <f>C24</f>
         <v>10</v>
       </c>
-      <c r="E24" s="48">
+      <c r="E24" s="44">
         <v>10</v>
       </c>
-      <c r="F24" s="50">
+      <c r="F24" s="46">
         <f>E24</f>
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="81" t="s">
+    <row r="25" spans="1:6" s="28" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="75" t="s">
         <v>79</v>
       </c>
-      <c r="B25" s="65" t="s">
+      <c r="B25" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="53">
+      <c r="C25" s="49">
         <v>0</v>
       </c>
-      <c r="D25" s="84">
+      <c r="D25" s="113">
         <f>(1-(1-C26)*C25)*(1-C27)</f>
         <v>1</v>
       </c>
-      <c r="E25" s="31">
+      <c r="E25" s="27">
         <v>0</v>
       </c>
-      <c r="F25" s="84">
+      <c r="F25" s="113">
         <f>(1-(1-E26)*E25)*(1-E27)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="82"/>
-      <c r="B26" s="65" t="s">
+    <row r="26" spans="1:6" s="28" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="76"/>
+      <c r="B26" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="53">
+      <c r="C26" s="49">
         <v>0.6</v>
       </c>
-      <c r="D26" s="85"/>
-      <c r="E26" s="31">
+      <c r="D26" s="114"/>
+      <c r="E26" s="27">
         <v>0.6</v>
       </c>
-      <c r="F26" s="85"/>
-    </row>
-    <row r="27" spans="1:6" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="83"/>
-      <c r="B27" s="65" t="s">
+      <c r="F26" s="114"/>
+    </row>
+    <row r="27" spans="1:6" s="28" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="77"/>
+      <c r="B27" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="55">
+      <c r="C27" s="51">
         <v>0</v>
       </c>
-      <c r="D27" s="86"/>
-      <c r="E27" s="34">
+      <c r="D27" s="115"/>
+      <c r="E27" s="30">
         <v>0</v>
       </c>
-      <c r="F27" s="86"/>
-    </row>
-    <row r="28" spans="1:6" s="46" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="87" t="s">
+      <c r="F27" s="115"/>
+    </row>
+    <row r="28" spans="1:6" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="116" t="s">
         <v>102</v>
       </c>
-      <c r="B28" s="88"/>
-      <c r="C28" s="61">
+      <c r="B28" s="117"/>
+      <c r="C28" s="57">
         <v>0</v>
       </c>
-      <c r="D28" s="51">
+      <c r="D28" s="47">
         <f>C28*0.5+1</f>
         <v>1</v>
       </c>
-      <c r="E28" s="45">
+      <c r="E28" s="41">
         <v>0</v>
       </c>
-      <c r="F28" s="51">
+      <c r="F28" s="47">
         <f>E28*0.5+1</f>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="73" t="s">
+      <c r="A29" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="74"/>
-      <c r="C29" s="75">
+      <c r="B29" s="108"/>
+      <c r="C29" s="109">
         <f>D2*D3*D4*D9*D10*D12*D16*D18*D20*D23/D24/D25*D28</f>
         <v>912882.68628480006</v>
       </c>
-      <c r="D29" s="76"/>
-      <c r="E29" s="75">
+      <c r="D29" s="110"/>
+      <c r="E29" s="109">
         <f>F2*F3*F4*F9*F10*F12*F16*F18*F20*F23/F24/F25*F28</f>
         <v>888806.21472719987</v>
       </c>
-      <c r="F29" s="76"/>
+      <c r="F29" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="F4:F8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="F20:F22"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E29:F29"/>
@@ -2767,6 +3779,30 @@
     <mergeCell ref="D25:D27"/>
     <mergeCell ref="F25:F27"/>
     <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="F4:F8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FIX - Main workbook compatibility issue (IFS)
</commit_message>
<xml_diff>
--- a/Brainstorm.xlsx
+++ b/Brainstorm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal@SSD\Game\DL\dragalia-data-track\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51FCD06-345B-4330-9845-CF20BC739982}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D54DC90-750E-4024-9DA6-9983A9C5CE7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1665" windowWidth="20385" windowHeight="14535" xr2:uid="{4CFB4A6A-60C6-4091-BCA5-480044B61D33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4CFB4A6A-60C6-4091-BCA5-480044B61D33}"/>
   </bookViews>
   <sheets>
     <sheet name="Rotation" sheetId="8" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="148">
   <si>
     <t>睡抗</t>
   </si>
@@ -530,7 +530,13 @@
     <t>P2</t>
   </si>
   <si>
-    <t>Catherine</t>
+    <t>Cassandra</t>
+  </si>
+  <si>
+    <t>Yuya</t>
+  </si>
+  <si>
+    <t>Serena</t>
   </si>
 </sst>
 </file>
@@ -1400,6 +1406,42 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="5" fillId="35" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="35" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="4" fontId="5" fillId="23" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1415,136 +1457,100 @@
     <xf numFmtId="4" fontId="5" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="5" fillId="30" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="30" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="30" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="32" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="32" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="21" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="35" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="35" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="30" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="30" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="30" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="32" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="32" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1899,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B260D6A6-975E-4594-902D-33C279C7CA35}">
   <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2006,7 +2012,7 @@
         <v>87</v>
       </c>
       <c r="R2" s="66">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="S2" s="60" t="s">
         <v>9</v>
@@ -2017,7 +2023,7 @@
       </c>
       <c r="V2" s="69">
         <f>VLOOKUP(T3,$H$3:$M$13,6,FALSE)</f>
-        <v>2028</v>
+        <v>1600</v>
       </c>
       <c r="X2" s="57" t="s">
         <v>40</v>
@@ -2053,27 +2059,27 @@
       </c>
       <c r="I3" s="61">
         <f>B3 * (1+SUM($R:$R))</f>
-        <v>195</v>
+        <v>150</v>
       </c>
       <c r="J3" s="61">
         <f t="shared" ref="J3:J13" si="0">C3 * (1+SUM($R:$R))</f>
-        <v>390</v>
+        <v>300</v>
       </c>
       <c r="K3" s="61">
         <f t="shared" ref="K3:M10" si="1">D3 * (1+SUM($R:$R))</f>
-        <v>644.80000000000007</v>
+        <v>496</v>
       </c>
       <c r="L3" s="61">
         <f t="shared" si="1"/>
-        <v>989.30000000000007</v>
+        <v>761</v>
       </c>
       <c r="M3" s="61">
         <f t="shared" si="1"/>
-        <v>1497.6000000000001</v>
+        <v>1152</v>
       </c>
       <c r="N3" s="58">
         <f t="shared" ref="N3:N13" si="2">G3 * (1+SUM($R:$R))</f>
-        <v>448.5</v>
+        <v>345</v>
       </c>
       <c r="O3" s="72" t="s">
         <v>17</v>
@@ -2091,14 +2097,14 @@
         <v>77</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="U3" s="68" t="s">
         <v>102</v>
       </c>
       <c r="V3" s="69">
         <f>MOD(T6, V2)</f>
-        <v>1789</v>
+        <v>890</v>
       </c>
       <c r="W3" s="57" t="s">
         <v>39</v>
@@ -2139,27 +2145,27 @@
       </c>
       <c r="I4" s="61">
         <f t="shared" ref="I4:I13" si="3">B4 * (1+SUM($R:$R))</f>
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="J4" s="61">
         <f t="shared" si="0"/>
-        <v>338</v>
+        <v>260</v>
       </c>
       <c r="K4" s="61">
         <f t="shared" si="1"/>
-        <v>624</v>
+        <v>480</v>
       </c>
       <c r="L4" s="61">
         <f t="shared" si="1"/>
-        <v>1092</v>
+        <v>840</v>
       </c>
       <c r="M4" s="61">
         <f t="shared" si="1"/>
-        <v>2262</v>
+        <v>1740</v>
       </c>
       <c r="N4" s="58">
         <f t="shared" si="2"/>
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="O4" s="72" t="s">
         <v>88</v>
@@ -2171,20 +2177,20 @@
         <v>88</v>
       </c>
       <c r="R4" s="66">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="S4" s="60" t="s">
         <v>97</v>
       </c>
       <c r="T4" s="13">
-        <v>3817</v>
+        <v>2490</v>
       </c>
       <c r="U4" s="68" t="s">
         <v>103</v>
       </c>
       <c r="V4" s="69">
         <f>MOD(T7, V2)</f>
-        <v>1680</v>
+        <v>1109</v>
       </c>
       <c r="W4" s="57" t="s">
         <v>105</v>
@@ -2225,27 +2231,27 @@
       </c>
       <c r="I5" s="61">
         <f t="shared" si="3"/>
-        <v>187.20000000000002</v>
+        <v>144</v>
       </c>
       <c r="J5" s="61">
         <f t="shared" si="0"/>
-        <v>374.40000000000003</v>
+        <v>288</v>
       </c>
       <c r="K5" s="61">
         <f t="shared" si="1"/>
-        <v>717.6</v>
+        <v>552</v>
       </c>
       <c r="L5" s="61">
         <f t="shared" si="1"/>
-        <v>1092</v>
+        <v>840</v>
       </c>
       <c r="M5" s="61">
         <f t="shared" si="1"/>
-        <v>1716</v>
+        <v>1320</v>
       </c>
       <c r="N5" s="58">
         <f t="shared" si="2"/>
-        <v>374.40000000000003</v>
+        <v>288</v>
       </c>
       <c r="O5" s="72" t="s">
         <v>89</v>
@@ -2263,14 +2269,14 @@
         <v>99</v>
       </c>
       <c r="T5" s="13">
-        <v>5736</v>
+        <v>5909</v>
       </c>
       <c r="U5" s="70" t="s">
         <v>100</v>
       </c>
       <c r="V5" s="71" t="str" cm="1">
         <f t="array" ref="V5">(ROUNDDOWN(T6/V2, 0) + IF(X8,1,0)) &amp; _xlfn.IFS(X3, " + FS", X4, " + C1", X5, " + C2", X6, " + C3", X7, " + C4", TRUE, "")</f>
-        <v>2</v>
+        <v>1 + C4</v>
       </c>
       <c r="W5" s="57" t="s">
         <v>106</v>
@@ -2311,41 +2317,41 @@
       </c>
       <c r="I6" s="61">
         <f t="shared" si="3"/>
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="J6" s="61">
         <f t="shared" si="0"/>
-        <v>572</v>
+        <v>440</v>
       </c>
       <c r="K6" s="61">
         <f t="shared" si="1"/>
-        <v>1040</v>
+        <v>800</v>
       </c>
       <c r="L6" s="61">
         <f t="shared" si="1"/>
-        <v>1534</v>
+        <v>1180</v>
       </c>
       <c r="M6" s="61">
         <f t="shared" si="1"/>
-        <v>2080</v>
+        <v>1600</v>
       </c>
       <c r="N6" s="58">
         <f t="shared" si="2"/>
-        <v>390</v>
+        <v>300</v>
       </c>
       <c r="S6" s="75" t="s">
         <v>98</v>
       </c>
       <c r="T6" s="76">
         <f>T4 * (1 - SUM(P:P))</f>
-        <v>3817</v>
+        <v>2490</v>
       </c>
       <c r="U6" s="77" t="s">
         <v>101</v>
       </c>
       <c r="V6" s="71" t="str" cm="1">
         <f t="array" ref="V6">(ROUNDDOWN(T7/V2, 0) + IF(Y8,1,0)) &amp; _xlfn.IFS(Y3, " + FS", Y4, " + C1", Y5, " + C2", Y6, " + C3", Y7, " + C4", TRUE, "")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W6" s="57" t="s">
         <v>107</v>
@@ -2386,41 +2392,41 @@
       </c>
       <c r="I7" s="61">
         <f t="shared" si="3"/>
-        <v>156</v>
+        <v>120</v>
       </c>
       <c r="J7" s="61">
         <f t="shared" si="0"/>
-        <v>468</v>
+        <v>360</v>
       </c>
       <c r="K7" s="61">
         <f t="shared" si="1"/>
-        <v>624</v>
+        <v>480</v>
       </c>
       <c r="L7" s="61">
         <f t="shared" si="1"/>
-        <v>1248</v>
+        <v>960</v>
       </c>
       <c r="M7" s="61">
         <f t="shared" si="1"/>
-        <v>2028</v>
+        <v>1560</v>
       </c>
       <c r="N7" s="58">
         <f t="shared" si="2"/>
-        <v>520</v>
+        <v>400</v>
       </c>
       <c r="S7" s="75" t="s">
         <v>104</v>
       </c>
       <c r="T7" s="76">
         <f>T5 * (1 - SUM(P:P))</f>
-        <v>5736</v>
+        <v>5909</v>
       </c>
       <c r="W7" s="57" t="s">
         <v>108</v>
       </c>
       <c r="X7" s="57" t="b">
         <f>AND(V3 &gt; VLOOKUP($T$3,$H$3:$M$13,4,FALSE),V3 &lt;= VLOOKUP($T$3,$H$3:$M$13,5,FALSE))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y7" s="57" t="b">
         <f>AND(V4 &gt; VLOOKUP($T$3,$H$3:$M$13,4,FALSE),V4 &lt;= VLOOKUP($T$3,$H$3:$M$13,5,FALSE))</f>
@@ -2454,34 +2460,34 @@
       </c>
       <c r="I8" s="61">
         <f t="shared" si="3"/>
-        <v>239.20000000000002</v>
+        <v>184</v>
       </c>
       <c r="J8" s="61">
         <f t="shared" si="0"/>
-        <v>358.8</v>
+        <v>276</v>
       </c>
       <c r="K8" s="61">
         <f t="shared" si="1"/>
-        <v>717.6</v>
+        <v>552</v>
       </c>
       <c r="L8" s="61">
         <f t="shared" si="1"/>
-        <v>1255.8</v>
+        <v>966</v>
       </c>
       <c r="M8" s="61">
         <f t="shared" si="1"/>
-        <v>1943.5</v>
+        <v>1495</v>
       </c>
       <c r="N8" s="58">
         <f t="shared" si="2"/>
-        <v>598</v>
+        <v>460</v>
       </c>
       <c r="W8" s="57" t="s">
         <v>109</v>
       </c>
       <c r="X8" s="57" t="b">
         <f>V3&gt;VLOOKUP($T$3,$H$3:$M$13,5,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y8" s="57" t="b">
         <f>V4&gt;VLOOKUP($T$3,$H$3:$M$13,5,FALSE)</f>
@@ -2515,27 +2521,27 @@
       </c>
       <c r="I9" s="61">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="J9" s="61">
         <f t="shared" si="0"/>
-        <v>429</v>
+        <v>330</v>
       </c>
       <c r="K9" s="61">
         <f t="shared" si="1"/>
-        <v>741</v>
+        <v>570</v>
       </c>
       <c r="L9" s="61">
         <f t="shared" si="1"/>
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="M9" s="61">
         <f t="shared" si="1"/>
-        <v>2080</v>
+        <v>1600</v>
       </c>
       <c r="N9" s="58">
         <f t="shared" si="2"/>
-        <v>520</v>
+        <v>400</v>
       </c>
       <c r="W9" s="57"/>
       <c r="X9" s="57"/>
@@ -2568,27 +2574,27 @@
       </c>
       <c r="I10" s="61">
         <f t="shared" si="3"/>
-        <v>301.60000000000002</v>
+        <v>232</v>
       </c>
       <c r="J10" s="61">
         <f t="shared" si="0"/>
-        <v>603.20000000000005</v>
+        <v>464</v>
       </c>
       <c r="K10" s="61">
         <f t="shared" si="1"/>
-        <v>1055.6000000000001</v>
+        <v>812</v>
       </c>
       <c r="L10" s="61">
         <f t="shared" si="1"/>
-        <v>1658.8</v>
+        <v>1276</v>
       </c>
       <c r="M10" s="61">
         <f t="shared" si="1"/>
-        <v>2563.6</v>
+        <v>1972</v>
       </c>
       <c r="N10" s="58">
         <f t="shared" si="2"/>
-        <v>754</v>
+        <v>580</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2612,18 +2618,18 @@
       </c>
       <c r="I11" s="61">
         <f t="shared" si="3"/>
-        <v>708.5</v>
+        <v>545</v>
       </c>
       <c r="J11" s="61">
         <f t="shared" si="0"/>
-        <v>1417</v>
+        <v>1090</v>
       </c>
       <c r="K11" s="61"/>
       <c r="L11" s="61"/>
       <c r="M11" s="61"/>
       <c r="N11" s="58">
         <f t="shared" si="2"/>
-        <v>520</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2647,18 +2653,18 @@
       </c>
       <c r="I12" s="61">
         <f t="shared" si="3"/>
-        <v>603.20000000000005</v>
+        <v>464</v>
       </c>
       <c r="J12" s="61">
         <f t="shared" si="0"/>
-        <v>1206.4000000000001</v>
+        <v>928</v>
       </c>
       <c r="K12" s="61"/>
       <c r="L12" s="61"/>
       <c r="M12" s="61"/>
       <c r="N12" s="58">
         <f t="shared" si="2"/>
-        <v>520</v>
+        <v>400</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2684,21 +2690,21 @@
       </c>
       <c r="I13" s="61">
         <f t="shared" si="3"/>
-        <v>390</v>
+        <v>300</v>
       </c>
       <c r="J13" s="61">
         <f t="shared" si="0"/>
-        <v>993.2</v>
+        <v>764</v>
       </c>
       <c r="K13" s="61">
         <f>D13 * (1+SUM($R:$R))</f>
-        <v>1596.4</v>
+        <v>1228</v>
       </c>
       <c r="L13" s="61"/>
       <c r="M13" s="61"/>
       <c r="N13" s="58">
         <f t="shared" si="2"/>
-        <v>520</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -3651,11 +3657,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFF6CA3-18A6-4987-88AD-5768B35D8A0C}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I9" sqref="I9"/>
+      <selection pane="topRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3668,38 +3674,32 @@
     <col min="6" max="6" width="11.28515625" style="20" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="20"/>
     <col min="8" max="8" width="11.28515625" style="20" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="20"/>
-    <col min="10" max="10" width="11.28515625" style="20" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="20"/>
+    <col min="9" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="142" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="104" t="s">
+      <c r="B1" s="143"/>
+      <c r="C1" s="105" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="106"/>
+      <c r="E1" s="105" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="106"/>
+      <c r="G1" s="105" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="105"/>
-      <c r="E1" s="104" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" s="105"/>
-      <c r="G1" s="104" t="s">
-        <v>145</v>
-      </c>
-      <c r="H1" s="105"/>
-      <c r="I1" s="104" t="s">
-        <v>145</v>
-      </c>
-      <c r="J1" s="105"/>
-    </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
+      <c r="H1" s="106"/>
+    </row>
+    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="103"/>
+      <c r="B2" s="120"/>
       <c r="C2" s="21">
         <f>5/3</f>
         <v>1.6666666666666667</v>
@@ -3724,20 +3724,12 @@
         <f>G2</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="I2" s="21">
-        <f>5/3</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="J2" s="22">
-        <f>I2</f>
-        <v>1.6666666666666667</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="102" t="s">
+    </row>
+    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="103"/>
+      <c r="B3" s="120"/>
       <c r="C3" s="21">
         <v>0</v>
       </c>
@@ -3759,175 +3751,137 @@
         <f>1-G3</f>
         <v>1</v>
       </c>
-      <c r="I3" s="21">
-        <v>0</v>
-      </c>
-      <c r="J3" s="22">
-        <f>1-I3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="116" t="s">
+    </row>
+    <row r="4" spans="1:8" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="123" t="s">
         <v>60</v>
       </c>
       <c r="B4" s="45" t="s">
         <v>63</v>
       </c>
       <c r="C4" s="24">
-        <v>1003</v>
-      </c>
-      <c r="D4" s="95">
+        <v>5092</v>
+      </c>
+      <c r="D4" s="107">
         <f>(C4/(1+C5)*(1+C5+C6)*(1+C7)*(1+C8))</f>
-        <v>1003</v>
+        <v>5092</v>
       </c>
       <c r="E4" s="24">
-        <v>1003</v>
-      </c>
-      <c r="F4" s="95">
+        <v>4353</v>
+      </c>
+      <c r="F4" s="107">
         <f>(E4/(1+E5)*(1+E5+E6)*(1+E7)*(1+E8))</f>
-        <v>1133.3899999999999</v>
+        <v>5005.95</v>
       </c>
       <c r="G4" s="24">
-        <v>1003</v>
-      </c>
-      <c r="H4" s="95">
+        <v>4353</v>
+      </c>
+      <c r="H4" s="107">
         <f>(G4/(1+G5)*(1+G5+G6)*(1+G7)*(1+G8))</f>
-        <v>1003</v>
-      </c>
-      <c r="I4" s="24">
-        <v>1003</v>
-      </c>
-      <c r="J4" s="95">
-        <f>(I4/(1+I5)*(1+I5+I6)*(1+I7)*(1+I8))</f>
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="117"/>
+        <v>5005.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="124"/>
       <c r="B5" s="45" t="s">
         <v>44</v>
       </c>
       <c r="C5" s="26">
         <v>0</v>
       </c>
-      <c r="D5" s="96"/>
+      <c r="D5" s="108"/>
       <c r="E5" s="26">
         <v>0</v>
       </c>
-      <c r="F5" s="96"/>
+      <c r="F5" s="108"/>
       <c r="G5" s="26">
         <v>0</v>
       </c>
-      <c r="H5" s="96"/>
-      <c r="I5" s="26">
-        <v>0</v>
-      </c>
-      <c r="J5" s="96"/>
-    </row>
-    <row r="6" spans="1:10" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="117"/>
+      <c r="H5" s="108"/>
+    </row>
+    <row r="6" spans="1:8" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="124"/>
       <c r="B6" s="45" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="27">
         <v>0</v>
       </c>
-      <c r="D6" s="96"/>
+      <c r="D6" s="108"/>
       <c r="E6" s="27">
-        <v>0.13</v>
-      </c>
-      <c r="F6" s="96"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="108"/>
       <c r="G6" s="27">
         <v>0</v>
       </c>
-      <c r="H6" s="96"/>
-      <c r="I6" s="27">
-        <v>0</v>
-      </c>
-      <c r="J6" s="96"/>
-    </row>
-    <row r="7" spans="1:10" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="117"/>
+      <c r="H6" s="108"/>
+    </row>
+    <row r="7" spans="1:8" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="124"/>
       <c r="B7" s="45" t="s">
         <v>56</v>
       </c>
       <c r="C7" s="27">
         <v>0</v>
       </c>
-      <c r="D7" s="96"/>
+      <c r="D7" s="108"/>
       <c r="E7" s="27">
-        <v>0</v>
-      </c>
-      <c r="F7" s="96"/>
+        <v>0.15</v>
+      </c>
+      <c r="F7" s="108"/>
       <c r="G7" s="27">
-        <v>0</v>
-      </c>
-      <c r="H7" s="96"/>
-      <c r="I7" s="27">
-        <v>0</v>
-      </c>
-      <c r="J7" s="96"/>
-    </row>
-    <row r="8" spans="1:10" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="118"/>
+        <v>0.15</v>
+      </c>
+      <c r="H7" s="108"/>
+    </row>
+    <row r="8" spans="1:8" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="125"/>
       <c r="B8" s="45" t="s">
         <v>57</v>
       </c>
       <c r="C8" s="27">
         <v>0</v>
       </c>
-      <c r="D8" s="97"/>
+      <c r="D8" s="109"/>
       <c r="E8" s="27">
         <v>0</v>
       </c>
-      <c r="F8" s="97"/>
+      <c r="F8" s="109"/>
       <c r="G8" s="27">
         <v>0</v>
       </c>
-      <c r="H8" s="97"/>
-      <c r="I8" s="27">
-        <v>0</v>
-      </c>
-      <c r="J8" s="97"/>
-    </row>
-    <row r="9" spans="1:10" s="30" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="119" t="s">
+      <c r="H8" s="109"/>
+    </row>
+    <row r="9" spans="1:8" s="30" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="138" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="120"/>
+      <c r="B9" s="139"/>
       <c r="C9" s="28">
-        <v>40.479999999999997</v>
+        <v>22.4</v>
       </c>
       <c r="D9" s="29">
         <f>C9</f>
-        <v>40.479999999999997</v>
+        <v>22.4</v>
       </c>
       <c r="E9" s="28">
-        <v>0.54</v>
+        <v>29.16</v>
       </c>
       <c r="F9" s="29">
         <f>E9</f>
-        <v>0.54</v>
+        <v>29.16</v>
       </c>
       <c r="G9" s="28">
-        <v>0.54</v>
+        <v>31.71</v>
       </c>
       <c r="H9" s="29">
         <f>G9</f>
-        <v>0.54</v>
-      </c>
-      <c r="I9" s="28">
-        <f>0.54*46</f>
-        <v>24.840000000000003</v>
-      </c>
-      <c r="J9" s="29">
-        <f>I9</f>
-        <v>24.840000000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="121" t="s">
+        <v>31.71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="140" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="46" t="s">
@@ -3936,158 +3890,128 @@
       <c r="C10" s="31">
         <v>0</v>
       </c>
-      <c r="D10" s="98">
+      <c r="D10" s="110">
         <f>1+((0.7+C11)*C10)</f>
         <v>1</v>
       </c>
       <c r="E10" s="31">
         <v>0</v>
       </c>
-      <c r="F10" s="98">
+      <c r="F10" s="110">
         <f>1+((0.7+E11)*E10)</f>
         <v>1</v>
       </c>
       <c r="G10" s="31">
         <v>0</v>
       </c>
-      <c r="H10" s="98">
+      <c r="H10" s="110">
         <f>1+((0.7+G11)*G10)</f>
         <v>1</v>
       </c>
-      <c r="I10" s="31">
-        <v>0</v>
-      </c>
-      <c r="J10" s="98">
-        <f>1+((0.7+I11)*I10)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="122"/>
+    </row>
+    <row r="11" spans="1:8" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="141"/>
       <c r="B11" s="46" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="33">
         <v>0</v>
       </c>
-      <c r="D11" s="99"/>
+      <c r="D11" s="111"/>
       <c r="E11" s="33">
         <v>0</v>
       </c>
-      <c r="F11" s="99"/>
+      <c r="F11" s="111"/>
       <c r="G11" s="33">
         <v>0</v>
       </c>
-      <c r="H11" s="99"/>
-      <c r="I11" s="33">
-        <v>0</v>
-      </c>
-      <c r="J11" s="99"/>
-    </row>
-    <row r="12" spans="1:10" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="111" t="s">
+      <c r="H11" s="111"/>
+    </row>
+    <row r="12" spans="1:8" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="133" t="s">
         <v>64</v>
       </c>
       <c r="B12" s="47" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="34">
-        <v>0.3</v>
-      </c>
-      <c r="D12" s="139">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="112">
         <f>(1+C12+C13)*(1+C14)*(1+C15)</f>
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="E12" s="34">
-        <v>0.3</v>
-      </c>
-      <c r="F12" s="139">
+        <v>0</v>
+      </c>
+      <c r="F12" s="112">
         <f>(1+E12+E13)*(1+E14)*(1+E15)</f>
-        <v>1.3</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G12" s="34">
-        <v>0.3</v>
-      </c>
-      <c r="H12" s="139">
+        <v>0</v>
+      </c>
+      <c r="H12" s="112">
         <f>(1+G12+G13)*(1+G14)*(1+G15)</f>
-        <v>1.3</v>
-      </c>
-      <c r="I12" s="34">
-        <v>0.3</v>
-      </c>
-      <c r="J12" s="139">
-        <f>(1+I12+I13)*(1+I14)*(1+I15)</f>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="112"/>
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="134"/>
       <c r="B13" s="47" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="34">
         <v>0</v>
       </c>
-      <c r="D13" s="140"/>
+      <c r="D13" s="113"/>
       <c r="E13" s="34">
         <v>0</v>
       </c>
-      <c r="F13" s="140"/>
+      <c r="F13" s="113"/>
       <c r="G13" s="34">
         <v>0</v>
       </c>
-      <c r="H13" s="140"/>
-      <c r="I13" s="34">
-        <v>0</v>
-      </c>
-      <c r="J13" s="140"/>
-    </row>
-    <row r="14" spans="1:10" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="112"/>
+      <c r="H13" s="113"/>
+    </row>
+    <row r="14" spans="1:8" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="134"/>
       <c r="B14" s="47" t="s">
         <v>69</v>
       </c>
       <c r="C14" s="34">
         <v>0</v>
       </c>
-      <c r="D14" s="140"/>
+      <c r="D14" s="113"/>
       <c r="E14" s="34">
-        <v>0</v>
-      </c>
-      <c r="F14" s="140"/>
+        <v>0.15</v>
+      </c>
+      <c r="F14" s="113"/>
       <c r="G14" s="34">
-        <v>0</v>
-      </c>
-      <c r="H14" s="140"/>
-      <c r="I14" s="34">
-        <v>0</v>
-      </c>
-      <c r="J14" s="140"/>
-    </row>
-    <row r="15" spans="1:10" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="113"/>
+        <v>0.15</v>
+      </c>
+      <c r="H14" s="113"/>
+    </row>
+    <row r="15" spans="1:8" s="35" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="135"/>
       <c r="B15" s="47" t="s">
         <v>70</v>
       </c>
       <c r="C15" s="34">
         <v>0</v>
       </c>
-      <c r="D15" s="141"/>
+      <c r="D15" s="114"/>
       <c r="E15" s="34">
         <v>0</v>
       </c>
-      <c r="F15" s="141"/>
+      <c r="F15" s="114"/>
       <c r="G15" s="34">
         <v>0</v>
       </c>
-      <c r="H15" s="141"/>
-      <c r="I15" s="34">
-        <v>0</v>
-      </c>
-      <c r="J15" s="141"/>
-    </row>
-    <row r="16" spans="1:10" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="114" t="s">
+      <c r="H15" s="114"/>
+    </row>
+    <row r="16" spans="1:8" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="136" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="48" t="s">
@@ -4096,56 +4020,45 @@
       <c r="C16" s="36">
         <v>0</v>
       </c>
-      <c r="D16" s="142">
+      <c r="D16" s="115">
         <f>(1+C16)*(1+C17)</f>
         <v>1</v>
       </c>
       <c r="E16" s="36">
         <v>0</v>
       </c>
-      <c r="F16" s="142">
+      <c r="F16" s="115">
         <f>(1+E16)*(1+E17)</f>
         <v>1</v>
       </c>
       <c r="G16" s="36">
         <v>0</v>
       </c>
-      <c r="H16" s="142">
+      <c r="H16" s="115">
         <f>(1+G16)*(1+G17)</f>
         <v>1</v>
       </c>
-      <c r="I16" s="36">
-        <v>0</v>
-      </c>
-      <c r="J16" s="142">
-        <f>(1+I16)*(1+I17)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="115"/>
+    </row>
+    <row r="17" spans="1:8" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="137"/>
       <c r="B17" s="48" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="36">
         <v>0</v>
       </c>
-      <c r="D17" s="143"/>
+      <c r="D17" s="116"/>
       <c r="E17" s="36">
         <v>0</v>
       </c>
-      <c r="F17" s="143"/>
+      <c r="F17" s="116"/>
       <c r="G17" s="36">
         <v>0</v>
       </c>
-      <c r="H17" s="143"/>
-      <c r="I17" s="36">
-        <v>0</v>
-      </c>
-      <c r="J17" s="143"/>
-    </row>
-    <row r="18" spans="1:10" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="106" t="s">
+      <c r="H17" s="116"/>
+    </row>
+    <row r="18" spans="1:8" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="128" t="s">
         <v>66</v>
       </c>
       <c r="B18" s="49" t="s">
@@ -4154,56 +4067,45 @@
       <c r="C18" s="38">
         <v>1.5</v>
       </c>
-      <c r="D18" s="129">
+      <c r="D18" s="95">
         <f>C18+C19</f>
         <v>1.5</v>
       </c>
       <c r="E18" s="38">
         <v>1.5</v>
       </c>
-      <c r="F18" s="129">
+      <c r="F18" s="95">
         <f>E18+E19</f>
         <v>1.5</v>
       </c>
       <c r="G18" s="38">
         <v>1.5</v>
       </c>
-      <c r="H18" s="129">
+      <c r="H18" s="95">
         <f>G18+G19</f>
         <v>1.5</v>
       </c>
-      <c r="I18" s="38">
-        <v>1.5</v>
-      </c>
-      <c r="J18" s="129">
-        <f>I18+I19</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="107"/>
+    </row>
+    <row r="19" spans="1:8" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="129"/>
       <c r="B19" s="49" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="40">
         <v>0</v>
       </c>
-      <c r="D19" s="130"/>
+      <c r="D19" s="96"/>
       <c r="E19" s="40">
         <v>0</v>
       </c>
-      <c r="F19" s="130"/>
+      <c r="F19" s="96"/>
       <c r="G19" s="40">
         <v>0</v>
       </c>
-      <c r="H19" s="130"/>
-      <c r="I19" s="40">
-        <v>0</v>
-      </c>
-      <c r="J19" s="130"/>
-    </row>
-    <row r="20" spans="1:10" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="108" t="s">
+      <c r="H19" s="96"/>
+    </row>
+    <row r="20" spans="1:8" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="130" t="s">
         <v>72</v>
       </c>
       <c r="B20" s="50" t="s">
@@ -4212,81 +4114,66 @@
       <c r="C20" s="41">
         <v>0</v>
       </c>
-      <c r="D20" s="131">
+      <c r="D20" s="97">
         <f>1+C20*(0.2+C21+C22)</f>
         <v>1</v>
       </c>
       <c r="E20" s="41">
         <v>0</v>
       </c>
-      <c r="F20" s="131">
+      <c r="F20" s="97">
         <f>1+E20*(0.2+E21+E22)</f>
         <v>1</v>
       </c>
       <c r="G20" s="41">
         <v>0</v>
       </c>
-      <c r="H20" s="131">
+      <c r="H20" s="97">
         <f>1+G20*(0.2+G21+G22)</f>
         <v>1</v>
       </c>
-      <c r="I20" s="41">
-        <v>0</v>
-      </c>
-      <c r="J20" s="131">
-        <f>1+I20*(0.2+I21+I22)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="109"/>
+    </row>
+    <row r="21" spans="1:8" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="131"/>
       <c r="B21" s="50" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="41">
         <v>0.5</v>
       </c>
-      <c r="D21" s="132"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="41">
         <v>0.5</v>
       </c>
-      <c r="F21" s="132"/>
+      <c r="F21" s="98"/>
       <c r="G21" s="41">
         <v>0.5</v>
       </c>
-      <c r="H21" s="132"/>
-      <c r="I21" s="41">
-        <v>0.5</v>
-      </c>
-      <c r="J21" s="132"/>
-    </row>
-    <row r="22" spans="1:10" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="110"/>
+      <c r="H21" s="98"/>
+    </row>
+    <row r="22" spans="1:8" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="132"/>
       <c r="B22" s="50" t="s">
         <v>51</v>
       </c>
       <c r="C22" s="41">
         <v>0</v>
       </c>
-      <c r="D22" s="133"/>
+      <c r="D22" s="99"/>
       <c r="E22" s="41">
         <v>0</v>
       </c>
-      <c r="F22" s="133"/>
+      <c r="F22" s="99"/>
       <c r="G22" s="41">
         <v>0</v>
       </c>
-      <c r="H22" s="133"/>
-      <c r="I22" s="41">
-        <v>0</v>
-      </c>
-      <c r="J22" s="133"/>
-    </row>
-    <row r="23" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="102" t="s">
+      <c r="H22" s="99"/>
+    </row>
+    <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="119" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="103"/>
+      <c r="B23" s="120"/>
       <c r="C23" s="21">
         <v>1</v>
       </c>
@@ -4308,19 +4195,12 @@
         <f>G23</f>
         <v>1</v>
       </c>
-      <c r="I23" s="21">
-        <v>1</v>
-      </c>
-      <c r="J23" s="23">
-        <f>I23</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="125" t="s">
+    </row>
+    <row r="24" spans="1:8" s="42" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="121" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="126"/>
+      <c r="B24" s="122"/>
       <c r="C24" s="41">
         <v>10</v>
       </c>
@@ -4342,16 +4222,9 @@
         <f>G24</f>
         <v>10</v>
       </c>
-      <c r="I24" s="41">
-        <v>10</v>
-      </c>
-      <c r="J24" s="43">
-        <f>I24</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="116" t="s">
+    </row>
+    <row r="25" spans="1:8" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="123" t="s">
         <v>53</v>
       </c>
       <c r="B25" s="45" t="s">
@@ -4360,81 +4233,66 @@
       <c r="C25" s="24">
         <v>0</v>
       </c>
-      <c r="D25" s="134">
+      <c r="D25" s="100">
         <f>(1-(1-C26)*C25)*(1-C27)</f>
         <v>1</v>
       </c>
       <c r="E25" s="24">
         <v>0</v>
       </c>
-      <c r="F25" s="134">
+      <c r="F25" s="100">
         <f>(1-(1-E26)*E25)*(1-E27)</f>
         <v>1</v>
       </c>
       <c r="G25" s="24">
         <v>0</v>
       </c>
-      <c r="H25" s="134">
+      <c r="H25" s="100">
         <f>(1-(1-G26)*G25)*(1-G27)</f>
         <v>1</v>
       </c>
-      <c r="I25" s="24">
-        <v>0</v>
-      </c>
-      <c r="J25" s="134">
-        <f>(1-(1-I26)*I25)*(1-I27)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="117"/>
+    </row>
+    <row r="26" spans="1:8" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="124"/>
       <c r="B26" s="45" t="s">
         <v>74</v>
       </c>
       <c r="C26" s="24">
         <v>0.6</v>
       </c>
-      <c r="D26" s="135"/>
+      <c r="D26" s="101"/>
       <c r="E26" s="24">
         <v>0.6</v>
       </c>
-      <c r="F26" s="135"/>
+      <c r="F26" s="101"/>
       <c r="G26" s="24">
         <v>0.6</v>
       </c>
-      <c r="H26" s="135"/>
-      <c r="I26" s="24">
-        <v>0.6</v>
-      </c>
-      <c r="J26" s="135"/>
-    </row>
-    <row r="27" spans="1:10" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="118"/>
+      <c r="H26" s="101"/>
+    </row>
+    <row r="27" spans="1:8" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="125"/>
       <c r="B27" s="45" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="27">
         <v>0</v>
       </c>
-      <c r="D27" s="136"/>
+      <c r="D27" s="102"/>
       <c r="E27" s="27">
         <v>0</v>
       </c>
-      <c r="F27" s="136"/>
+      <c r="F27" s="102"/>
       <c r="G27" s="27">
         <v>0</v>
       </c>
-      <c r="H27" s="136"/>
-      <c r="I27" s="27">
-        <v>0</v>
-      </c>
-      <c r="J27" s="136"/>
-    </row>
-    <row r="28" spans="1:10" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="127" t="s">
+      <c r="H27" s="102"/>
+    </row>
+    <row r="28" spans="1:8" s="39" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="126" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="128"/>
+      <c r="B28" s="127"/>
       <c r="C28" s="38">
         <v>0</v>
       </c>
@@ -4456,106 +4314,56 @@
         <f>G28*0.5+1</f>
         <v>1</v>
       </c>
-      <c r="I28" s="38">
-        <v>0</v>
-      </c>
-      <c r="J28" s="44">
-        <f>I28*0.5+1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="123" t="s">
+    </row>
+    <row r="29" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="117" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="124"/>
-      <c r="C29" s="137">
+      <c r="B29" s="118"/>
+      <c r="C29" s="103">
         <f>D2*D3*D4*D9*D10*D12*D16*D18*D20*D23/D24/D25*D28</f>
-        <v>13195.467999999999</v>
-      </c>
-      <c r="D29" s="138"/>
-      <c r="E29" s="137">
+        <v>34218.240000000005</v>
+      </c>
+      <c r="D29" s="104"/>
+      <c r="E29" s="103">
         <f>F2*F3*F4*F9*F10*F12*F16*F18*F20*F23/F24/F25*F28</f>
-        <v>198.90994499999999</v>
-      </c>
-      <c r="F29" s="138"/>
-      <c r="G29" s="137">
+        <v>41967.381825000004</v>
+      </c>
+      <c r="F29" s="104"/>
+      <c r="G29" s="103">
         <f>H2*H3*H4*H9*H10*H12*H16*H18*H20*H23/H24/H25*H28</f>
-        <v>176.0265</v>
-      </c>
-      <c r="H29" s="138"/>
-      <c r="I29" s="137">
-        <f>J2*J3*J4*J9*J10*J12*J16*J18*J20*J23/J24/J25*J28</f>
-        <v>8097.2190000000001</v>
-      </c>
-      <c r="J29" s="138"/>
-    </row>
-    <row r="30" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45637.368918750006</v>
+      </c>
+      <c r="H29" s="104"/>
+    </row>
+    <row r="30" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="20" t="s">
         <v>138</v>
       </c>
       <c r="D30" s="20">
-        <v>124889</v>
+        <v>36488</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>138</v>
       </c>
       <c r="F30" s="20">
-        <v>124889</v>
+        <v>38700</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>138</v>
       </c>
       <c r="H30" s="20">
-        <v>124889</v>
-      </c>
-      <c r="I30" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="J30" s="20">
-        <v>124889</v>
+        <v>38700</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="F4:F8"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="H4:H8"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="J4:J8"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="H25:H27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:B28"/>
+  <mergeCells count="42">
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C1:D1"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A12:A15"/>
@@ -4563,12 +4371,35 @@
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="H4:H8"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="F4:F8"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FIX - Manacaster SP errors and others
</commit_message>
<xml_diff>
--- a/Brainstorm.xlsx
+++ b/Brainstorm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal@SSD\Game\DL\dragalia-data-track\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF584EC-869D-4DC5-BEB4-4F355483402C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B36A24F-1853-4806-B227-5294F2CAC183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9735" yWindow="1170" windowWidth="23205" windowHeight="13545" activeTab="5" xr2:uid="{4CFB4A6A-60C6-4091-BCA5-480044B61D33}"/>
+    <workbookView xWindow="29520" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{4CFB4A6A-60C6-4091-BCA5-480044B61D33}"/>
   </bookViews>
   <sheets>
     <sheet name="Rotation" sheetId="8" r:id="rId1"/>
@@ -351,12 +351,6 @@
     <t>長銃</t>
   </si>
   <si>
-    <t>短銃</t>
-  </si>
-  <si>
-    <t>散銃</t>
-  </si>
-  <si>
     <t>EX</t>
   </si>
   <si>
@@ -657,6 +651,12 @@
   </si>
   <si>
     <t>馬斯</t>
+  </si>
+  <si>
+    <t>機關</t>
+  </si>
+  <si>
+    <t>散彈</t>
   </si>
 </sst>
 </file>
@@ -2262,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B260D6A6-975E-4594-902D-33C279C7CA35}">
   <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2282,7 +2282,7 @@
   <sheetData>
     <row r="1" spans="1:25" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="131" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" s="132"/>
       <c r="C1" s="132"/>
@@ -2291,7 +2291,7 @@
       <c r="F1" s="132"/>
       <c r="G1" s="133"/>
       <c r="H1" s="131" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I1" s="132"/>
       <c r="J1" s="132"/>
@@ -2300,19 +2300,19 @@
       <c r="M1" s="132"/>
       <c r="N1" s="133"/>
       <c r="O1" s="134" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P1" s="135"/>
       <c r="Q1" s="125" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R1" s="126"/>
       <c r="S1" s="127" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T1" s="128"/>
       <c r="U1" s="129" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="V1" s="130"/>
     </row>
@@ -2321,19 +2321,19 @@
         <v>16</v>
       </c>
       <c r="B2" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="E2" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="F2" s="62" t="s">
         <v>107</v>
-      </c>
-      <c r="E2" s="62" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="62" t="s">
-        <v>109</v>
       </c>
       <c r="G2" s="63" t="s">
         <v>39</v>
@@ -2342,45 +2342,45 @@
         <v>16</v>
       </c>
       <c r="I2" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="J2" s="62" t="s">
+      <c r="L2" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="K2" s="62" t="s">
+      <c r="M2" s="62" t="s">
         <v>107</v>
-      </c>
-      <c r="L2" s="62" t="s">
-        <v>108</v>
-      </c>
-      <c r="M2" s="62" t="s">
-        <v>109</v>
       </c>
       <c r="N2" s="63" t="s">
         <v>39</v>
       </c>
       <c r="O2" s="72" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P2" s="73">
         <v>0</v>
       </c>
       <c r="Q2" s="59" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="R2" s="66">
-        <v>0.23</v>
+        <v>0.15</v>
       </c>
       <c r="S2" s="60" t="s">
         <v>9</v>
       </c>
       <c r="T2" s="12"/>
       <c r="U2" s="68" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="V2" s="69">
         <f>VLOOKUP(T3,$H$3:$M$13,6,FALSE)</f>
-        <v>2911.9999999999995</v>
+        <v>2064</v>
       </c>
       <c r="X2" s="57" t="s">
         <v>40</v>
@@ -2416,27 +2416,27 @@
       </c>
       <c r="I3" s="61">
         <f>B3 * (1+SUM($R:$R))</f>
-        <v>273</v>
+        <v>193.5</v>
       </c>
       <c r="J3" s="61">
         <f t="shared" ref="J3:J13" si="0">C3 * (1+SUM($R:$R))</f>
-        <v>546</v>
+        <v>387</v>
       </c>
       <c r="K3" s="61">
         <f t="shared" ref="K3:M10" si="1">D3 * (1+SUM($R:$R))</f>
-        <v>902.71999999999991</v>
+        <v>639.84</v>
       </c>
       <c r="L3" s="61">
         <f t="shared" si="1"/>
-        <v>1385.02</v>
+        <v>981.69</v>
       </c>
       <c r="M3" s="61">
         <f t="shared" si="1"/>
-        <v>2096.64</v>
+        <v>1486.08</v>
       </c>
       <c r="N3" s="58">
         <f t="shared" ref="N3:N13" si="2">G3 * (1+SUM($R:$R))</f>
-        <v>627.9</v>
+        <v>445.05</v>
       </c>
       <c r="O3" s="72" t="s">
         <v>17</v>
@@ -2448,7 +2448,7 @@
         <v>17</v>
       </c>
       <c r="R3" s="66">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="S3" s="60" t="s">
         <v>77</v>
@@ -2457,22 +2457,22 @@
         <v>29</v>
       </c>
       <c r="U3" s="68" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="V3" s="69">
         <f>MOD(T6, V2)</f>
-        <v>613.00000000000045</v>
+        <v>672</v>
       </c>
       <c r="W3" s="57" t="s">
         <v>39</v>
       </c>
       <c r="X3" s="57" t="b">
         <f>AND(V3 &gt; 0, V3 &lt;= VLOOKUP($T$3,$H$3:$N$13,7,FALSE))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y3" s="57" t="b">
         <f>AND(V4 &gt; 0, V4 &lt;= VLOOKUP($T$3,$H$3:$N$13,7,FALSE))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2502,55 +2502,55 @@
       </c>
       <c r="I4" s="61">
         <f t="shared" ref="I4:I13" si="3">B4 * (1+SUM($R:$R))</f>
-        <v>236.59999999999997</v>
+        <v>167.70000000000002</v>
       </c>
       <c r="J4" s="61">
         <f t="shared" si="0"/>
-        <v>473.19999999999993</v>
+        <v>335.40000000000003</v>
       </c>
       <c r="K4" s="61">
         <f t="shared" si="1"/>
-        <v>873.59999999999991</v>
+        <v>619.20000000000005</v>
       </c>
       <c r="L4" s="61">
         <f t="shared" si="1"/>
-        <v>1528.8</v>
+        <v>1083.6000000000001</v>
       </c>
       <c r="M4" s="61">
         <f t="shared" si="1"/>
-        <v>3166.7999999999997</v>
+        <v>2244.6</v>
       </c>
       <c r="N4" s="58">
         <f t="shared" si="2"/>
-        <v>363.99999999999994</v>
+        <v>258</v>
       </c>
       <c r="O4" s="72" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P4" s="73">
         <v>0</v>
       </c>
       <c r="Q4" s="59" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="R4" s="66">
         <v>0.14000000000000001</v>
       </c>
       <c r="S4" s="60" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="T4" s="13">
-        <v>3525</v>
+        <v>4800</v>
       </c>
       <c r="U4" s="68" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="V4" s="69">
         <f>MOD(T7, V2)</f>
-        <v>2499.0000000000018</v>
+        <v>85</v>
       </c>
       <c r="W4" s="57" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="X4" s="57" t="b">
         <f>AND(V3 &gt; VLOOKUP($T$3,$H$3:$M$13,1,FALSE),V3 &lt;= VLOOKUP($T$3,$H$3:$M$13,2,FALSE))</f>
@@ -2588,55 +2588,55 @@
       </c>
       <c r="I5" s="61">
         <f t="shared" si="3"/>
-        <v>262.08</v>
+        <v>185.76</v>
       </c>
       <c r="J5" s="61">
         <f t="shared" si="0"/>
-        <v>524.16</v>
+        <v>371.52</v>
       </c>
       <c r="K5" s="61">
         <f t="shared" si="1"/>
-        <v>1004.6399999999999</v>
+        <v>712.08</v>
       </c>
       <c r="L5" s="61">
         <f t="shared" si="1"/>
-        <v>1528.8</v>
+        <v>1083.6000000000001</v>
       </c>
       <c r="M5" s="61">
         <f t="shared" si="1"/>
-        <v>2402.3999999999996</v>
+        <v>1702.8</v>
       </c>
       <c r="N5" s="58">
         <f t="shared" si="2"/>
-        <v>524.16</v>
+        <v>371.52</v>
       </c>
       <c r="O5" s="72" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="P5" s="73">
         <v>0</v>
       </c>
       <c r="Q5" s="59" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="R5" s="66">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="S5" s="60" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="T5" s="13">
-        <v>14147</v>
+        <v>8341</v>
       </c>
       <c r="U5" s="70" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="V5" s="71" t="str" cm="1">
         <f t="array" ref="V5">(ROUNDDOWN(T6/V2, 0) + IF(X8,1,0)) &amp; _xlfn.IFS(X3, " + FS", X4, " + C1", X5, " + C2", X6, " + C3", X7, " + C4", TRUE, "")</f>
-        <v>1 + FS</v>
+        <v>2 + C3</v>
       </c>
       <c r="W5" s="57" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="X5" s="57" t="b">
         <f>AND(V3&gt;VLOOKUP($T$3,$H$3:$M$13,2,FALSE),V3&lt;=VLOOKUP($T$3,$H$3:$M$13,3,FALSE))</f>
@@ -2674,44 +2674,44 @@
       </c>
       <c r="I6" s="61">
         <f t="shared" si="3"/>
-        <v>363.99999999999994</v>
+        <v>258</v>
       </c>
       <c r="J6" s="61">
         <f t="shared" si="0"/>
-        <v>800.8</v>
+        <v>567.6</v>
       </c>
       <c r="K6" s="61">
         <f t="shared" si="1"/>
-        <v>1455.9999999999998</v>
+        <v>1032</v>
       </c>
       <c r="L6" s="61">
         <f t="shared" si="1"/>
-        <v>2147.6</v>
+        <v>1522.2</v>
       </c>
       <c r="M6" s="61">
         <f t="shared" si="1"/>
-        <v>2911.9999999999995</v>
+        <v>2064</v>
       </c>
       <c r="N6" s="58">
         <f t="shared" si="2"/>
-        <v>546</v>
+        <v>387</v>
       </c>
       <c r="S6" s="75" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="T6" s="76">
         <f>T4 * (1 - SUM(P:P))</f>
-        <v>3525</v>
+        <v>4800</v>
       </c>
       <c r="U6" s="77" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="V6" s="71" t="str" cm="1">
         <f t="array" ref="V6">(ROUNDDOWN(T7/V2, 0) + IF(Y8,1,0)) &amp; _xlfn.IFS(Y3, " + FS", Y4, " + C1", Y5, " + C2", Y6, " + C3", Y7, " + C4", TRUE, "")</f>
-        <v>5</v>
+        <v>4 + FS</v>
       </c>
       <c r="W6" s="57" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="X6" s="57" t="b">
         <f>AND(V3 &gt; VLOOKUP($T$3,$H$3:$M$13,3,FALSE),V3 &lt;= VLOOKUP($T$3,$H$3:$M$13,4,FALSE))</f>
@@ -2749,37 +2749,37 @@
       </c>
       <c r="I7" s="61">
         <f t="shared" si="3"/>
-        <v>218.39999999999998</v>
+        <v>154.80000000000001</v>
       </c>
       <c r="J7" s="61">
         <f t="shared" si="0"/>
-        <v>655.19999999999993</v>
+        <v>464.40000000000003</v>
       </c>
       <c r="K7" s="61">
         <f t="shared" si="1"/>
-        <v>873.59999999999991</v>
+        <v>619.20000000000005</v>
       </c>
       <c r="L7" s="61">
         <f t="shared" si="1"/>
-        <v>1747.1999999999998</v>
+        <v>1238.4000000000001</v>
       </c>
       <c r="M7" s="61">
         <f t="shared" si="1"/>
-        <v>2839.2</v>
+        <v>2012.4</v>
       </c>
       <c r="N7" s="58">
         <f t="shared" si="2"/>
-        <v>727.99999999999989</v>
+        <v>516</v>
       </c>
       <c r="S7" s="75" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T7" s="76">
         <f>T5 * (1 - SUM(P:P))</f>
-        <v>14147</v>
+        <v>8341</v>
       </c>
       <c r="W7" s="57" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="X7" s="57" t="b">
         <f>AND(V3 &gt; VLOOKUP($T$3,$H$3:$M$13,4,FALSE),V3 &lt;= VLOOKUP($T$3,$H$3:$M$13,5,FALSE))</f>
@@ -2817,30 +2817,30 @@
       </c>
       <c r="I8" s="61">
         <f t="shared" si="3"/>
-        <v>334.88</v>
+        <v>237.36</v>
       </c>
       <c r="J8" s="61">
         <f t="shared" si="0"/>
-        <v>502.31999999999994</v>
+        <v>356.04</v>
       </c>
       <c r="K8" s="61">
         <f t="shared" si="1"/>
-        <v>1004.6399999999999</v>
+        <v>712.08</v>
       </c>
       <c r="L8" s="61">
         <f t="shared" si="1"/>
-        <v>1758.12</v>
+        <v>1246.1400000000001</v>
       </c>
       <c r="M8" s="61">
         <f t="shared" si="1"/>
-        <v>2720.8999999999996</v>
+        <v>1928.55</v>
       </c>
       <c r="N8" s="58">
         <f t="shared" si="2"/>
-        <v>837.19999999999993</v>
+        <v>593.4</v>
       </c>
       <c r="W8" s="57" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="X8" s="57" t="b">
         <f>V3&gt;VLOOKUP($T$3,$H$3:$M$13,5,FALSE)</f>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="Y8" s="57" t="b">
         <f>V4&gt;VLOOKUP($T$3,$H$3:$M$13,5,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2878,27 +2878,27 @@
       </c>
       <c r="I9" s="61">
         <f t="shared" si="3"/>
-        <v>236.59999999999997</v>
+        <v>167.70000000000002</v>
       </c>
       <c r="J9" s="61">
         <f t="shared" si="0"/>
-        <v>600.59999999999991</v>
+        <v>425.7</v>
       </c>
       <c r="K9" s="61">
         <f t="shared" si="1"/>
-        <v>1037.3999999999999</v>
+        <v>735.30000000000007</v>
       </c>
       <c r="L9" s="61">
         <f t="shared" si="1"/>
-        <v>1819.9999999999998</v>
+        <v>1290</v>
       </c>
       <c r="M9" s="61">
         <f t="shared" si="1"/>
-        <v>2911.9999999999995</v>
+        <v>2064</v>
       </c>
       <c r="N9" s="58">
         <f t="shared" si="2"/>
-        <v>727.99999999999989</v>
+        <v>516</v>
       </c>
       <c r="W9" s="57"/>
       <c r="X9" s="57"/>
@@ -2931,27 +2931,27 @@
       </c>
       <c r="I10" s="61">
         <f t="shared" si="3"/>
-        <v>422.23999999999995</v>
+        <v>299.28000000000003</v>
       </c>
       <c r="J10" s="61">
         <f t="shared" si="0"/>
-        <v>844.4799999999999</v>
+        <v>598.56000000000006</v>
       </c>
       <c r="K10" s="61">
         <f t="shared" si="1"/>
-        <v>1477.84</v>
+        <v>1047.48</v>
       </c>
       <c r="L10" s="61">
         <f t="shared" si="1"/>
-        <v>2322.3199999999997</v>
+        <v>1646.04</v>
       </c>
       <c r="M10" s="61">
         <f t="shared" si="1"/>
-        <v>3589.0399999999995</v>
+        <v>2543.88</v>
       </c>
       <c r="N10" s="58">
         <f t="shared" si="2"/>
-        <v>1055.5999999999999</v>
+        <v>748.2</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2975,29 +2975,29 @@
       </c>
       <c r="I11" s="61">
         <f t="shared" si="3"/>
-        <v>991.89999999999986</v>
+        <v>703.05000000000007</v>
       </c>
       <c r="J11" s="61">
         <f t="shared" si="0"/>
-        <v>1983.7999999999997</v>
+        <v>1406.1000000000001</v>
       </c>
       <c r="K11" s="61"/>
       <c r="L11" s="61"/>
       <c r="M11" s="61"/>
       <c r="N11" s="58">
         <f t="shared" si="2"/>
-        <v>727.99999999999989</v>
+        <v>516</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>85</v>
+        <v>186</v>
       </c>
       <c r="B12" s="61">
-        <v>464</v>
+        <v>340</v>
       </c>
       <c r="C12" s="61">
-        <v>928</v>
+        <v>680</v>
       </c>
       <c r="D12" s="61"/>
       <c r="E12" s="61"/>
@@ -3006,62 +3006,62 @@
         <v>400</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>85</v>
+        <v>186</v>
       </c>
       <c r="I12" s="61">
         <f t="shared" si="3"/>
-        <v>844.4799999999999</v>
+        <v>438.6</v>
       </c>
       <c r="J12" s="61">
         <f t="shared" si="0"/>
-        <v>1688.9599999999998</v>
+        <v>877.2</v>
       </c>
       <c r="K12" s="61"/>
       <c r="L12" s="61"/>
       <c r="M12" s="61"/>
       <c r="N12" s="58">
         <f t="shared" si="2"/>
-        <v>727.99999999999989</v>
+        <v>516</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>86</v>
+        <v>185</v>
       </c>
       <c r="B13" s="61">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C13" s="61">
-        <v>764</v>
+        <v>400</v>
       </c>
       <c r="D13" s="61">
-        <v>1228</v>
+        <v>600</v>
       </c>
       <c r="E13" s="61"/>
       <c r="F13" s="61"/>
       <c r="G13" s="58">
-        <v>400</v>
+        <v>90</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>86</v>
+        <v>185</v>
       </c>
       <c r="I13" s="61">
         <f t="shared" si="3"/>
-        <v>546</v>
+        <v>258</v>
       </c>
       <c r="J13" s="61">
         <f t="shared" si="0"/>
-        <v>1390.4799999999998</v>
+        <v>516</v>
       </c>
       <c r="K13" s="61">
         <f>D13 * (1+SUM($R:$R))</f>
-        <v>2234.9599999999996</v>
+        <v>774</v>
       </c>
       <c r="L13" s="61"/>
       <c r="M13" s="61"/>
       <c r="N13" s="58">
         <f t="shared" si="2"/>
-        <v>727.99999999999989</v>
+        <v>116.10000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3287,19 +3287,19 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>33</v>
@@ -3336,25 +3336,25 @@
         <v>17</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>17</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3362,25 +3362,25 @@
         <v>18</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>18</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3388,25 +3388,25 @@
         <v>19</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3414,25 +3414,25 @@
         <v>20</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3440,25 +3440,25 @@
         <v>21</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3466,25 +3466,25 @@
         <v>22</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3544,25 +3544,25 @@
         <v>25</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3612,25 +3612,25 @@
         <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3638,25 +3638,25 @@
         <v>32</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3667,10 +3667,10 @@
     </row>
     <row r="18" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B18" s="137" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C18" s="137"/>
       <c r="D18" s="137"/>
@@ -3678,10 +3678,10 @@
     </row>
     <row r="19" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B19" s="136" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C19" s="137"/>
       <c r="D19" s="137"/>
@@ -3689,10 +3689,10 @@
     </row>
     <row r="20" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B20" s="136" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C20" s="137"/>
       <c r="D20" s="137"/>
@@ -3733,19 +3733,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="79" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D1" s="79" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3792,7 +3792,7 @@
     </row>
     <row r="4" spans="1:24" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -3859,7 +3859,7 @@
     </row>
     <row r="7" spans="1:24" s="8" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -3889,10 +3889,10 @@
         <v>38</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N8" s="9" t="s">
         <v>35</v>
@@ -3927,7 +3927,7 @@
     </row>
     <row r="10" spans="1:24" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -3958,10 +3958,10 @@
         <v>38</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="N11" s="15" t="s">
         <v>35</v>
@@ -3995,7 +3995,7 @@
     </row>
     <row r="13" spans="1:24" s="15" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -4003,7 +4003,7 @@
     </row>
     <row r="14" spans="1:24" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -4040,15 +4040,15 @@
       </c>
       <c r="B1" s="145"/>
       <c r="C1" s="148" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D1" s="149"/>
       <c r="E1" s="148" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F1" s="149"/>
       <c r="G1" s="148" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H1" s="149"/>
     </row>
@@ -4695,19 +4695,19 @@
     </row>
     <row r="30" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D30" s="20">
         <v>11704</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F30" s="20">
         <v>38700</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H30" s="20">
         <v>38700</v>
@@ -4768,7 +4768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DD32DD-C8F1-4E13-B59E-D06F7BB09858}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
@@ -4782,13 +4782,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="81" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D1" s="81" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E1" s="98" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="82" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -4796,7 +4796,7 @@
         <v>60</v>
       </c>
       <c r="B2" s="82" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C2" s="83">
         <v>0.55000000000000004</v>
@@ -4810,7 +4810,7 @@
     </row>
     <row r="3" spans="1:5" s="82" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="82" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3" s="188">
         <v>0.2</v>
@@ -4820,7 +4820,7 @@
     </row>
     <row r="4" spans="1:5" s="121" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="121" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C4" s="196">
         <v>0</v>
@@ -4830,7 +4830,7 @@
     </row>
     <row r="5" spans="1:5" s="103" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="103" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C5" s="102">
         <v>0</v>
@@ -4844,10 +4844,10 @@
     </row>
     <row r="6" spans="1:5" s="84" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="84" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B6" s="84" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C6" s="85">
         <v>0.6</v>
@@ -4861,7 +4861,7 @@
     </row>
     <row r="7" spans="1:5" s="84" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="84" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C7" s="193">
         <v>0.55000000000000004</v>
@@ -4871,7 +4871,7 @@
     </row>
     <row r="8" spans="1:5" s="84" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="84" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C8" s="193">
         <v>0</v>
@@ -4881,7 +4881,7 @@
     </row>
     <row r="9" spans="1:5" s="100" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="100" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C9" s="99">
         <v>0</v>
@@ -4895,10 +4895,10 @@
     </row>
     <row r="10" spans="1:5" s="86" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="86" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B10" s="86" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" s="87">
         <v>0</v>
@@ -4912,7 +4912,7 @@
     </row>
     <row r="11" spans="1:5" s="86" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="86" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C11" s="194">
         <v>0</v>
@@ -4922,7 +4922,7 @@
     </row>
     <row r="12" spans="1:5" s="86" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="86" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C12" s="192">
         <v>0.5</v>
@@ -4932,10 +4932,10 @@
     </row>
     <row r="13" spans="1:5" s="88" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="88" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B13" s="88" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C13" s="191">
         <v>0</v>
@@ -4945,7 +4945,7 @@
     </row>
     <row r="14" spans="1:5" s="122" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="122" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C14" s="191">
         <v>0</v>
@@ -4955,7 +4955,7 @@
     </row>
     <row r="15" spans="1:5" s="88" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="88" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C15" s="191">
         <v>0</v>
@@ -4965,10 +4965,10 @@
     </row>
     <row r="16" spans="1:5" s="89" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="89" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B16" s="89" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C16" s="189">
         <v>1</v>
@@ -4978,7 +4978,7 @@
     </row>
     <row r="17" spans="1:5" s="89" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="89" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C17" s="190">
         <v>1</v>
@@ -4988,10 +4988,10 @@
     </row>
     <row r="18" spans="1:5" s="90" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="90" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B18" s="90" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C18" s="92">
         <f t="shared" ref="C18" si="0">(1+C2+$C3)*(1+$C4+C5)*(1+C10+$C11+$C12)*(1+$C13)*$C16</f>
@@ -5026,7 +5026,7 @@
     </row>
     <row r="20" spans="1:5" s="90" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="90" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C20" s="92">
         <f>(1+C2+$C3)*(1+$C4+C5)*(1+C6+$C7+$C14)*(1+$C8+C9)*(1+C10+$C11+$C12)*(1+$C15)*$C17</f>
@@ -5083,7 +5083,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:J16"/>
+      <selection activeCell="C9" sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5105,46 +5105,46 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="72" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B2" s="94">
         <v>0.12</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D2" s="95">
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="72" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B3" s="94">
-        <v>0.44</v>
+        <v>0</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D3" s="95">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="72" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B4" s="94">
         <f>B2+B3</f>
-        <v>0.56000000000000005</v>
+        <v>0.12</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D4" s="95">
         <f>D2+D3</f>
-        <v>1.6</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5155,60 +5155,60 @@
         <v>42</v>
       </c>
       <c r="C5" s="202" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D5" s="203"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C6" s="200">
         <f>1*(1-B2)+(1+D2)*(B2)</f>
-        <v>1.1559999999999999</v>
+        <v>1.204</v>
       </c>
       <c r="D6" s="201"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="65" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B7" s="96" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C7" s="200">
         <f>1*(1-B2)+(1+D4)*(B2)</f>
-        <v>1.1919999999999999</v>
+        <v>1.258</v>
       </c>
       <c r="D7" s="201"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="96" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C8" s="200">
         <f>1*(1-B4)+(1+D2)*(B4)</f>
-        <v>1.728</v>
+        <v>1.204</v>
       </c>
       <c r="D8" s="201"/>
       <c r="F8" s="97"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="96" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B9" s="96" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C9" s="200">
         <f>1*(1-B4)+(1+D4)*(B4)</f>
-        <v>1.8960000000000001</v>
+        <v>1.258</v>
       </c>
       <c r="D9" s="201"/>
     </row>
@@ -5252,42 +5252,42 @@
   <sheetData>
     <row r="1" spans="1:12" s="104" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="111" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B1" s="111">
         <v>3</v>
       </c>
       <c r="D1" s="111" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="111" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="111" t="s">
         <v>165</v>
       </c>
-      <c r="E1" s="111" t="s">
+      <c r="G1" s="111" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="111" t="s">
         <v>166</v>
       </c>
-      <c r="F1" s="111" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="H1" s="111" t="s">
-        <v>168</v>
-      </c>
       <c r="I1" s="111" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J1" s="112" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K1" s="116" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="L1" s="118" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="111" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B2" s="113">
         <v>0.09</v>
@@ -5330,7 +5330,7 @@
     </row>
     <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="111" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B3" s="105">
         <v>12.2</v>
@@ -5374,7 +5374,7 @@
     </row>
     <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="111" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B4" s="113">
         <v>0.3</v>
@@ -5456,7 +5456,7 @@
     </row>
     <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="104" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B6" s="97">
         <f>B2*B4</f>
@@ -5539,7 +5539,7 @@
     </row>
     <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="65" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B8" s="114">
         <v>3.9</v>
@@ -5584,7 +5584,7 @@
     </row>
     <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="65" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B9" s="115">
         <v>0.06</v>
@@ -5628,7 +5628,7 @@
     </row>
     <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B10" s="115">
         <v>0.3</v>
@@ -5711,7 +5711,7 @@
     </row>
     <row r="12" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="104" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B12" s="97">
         <f>B9*(1-B10)</f>
@@ -5756,7 +5756,7 @@
     </row>
     <row r="13" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="104" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B13" s="110">
         <f>B12/B8</f>

</xml_diff>